<commit_message>
TS 2 Files 15072019 from NMV
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="1142">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -2571,9 +2571,6 @@
     <t>yuvayOr yaH</t>
   </si>
   <si>
-    <t>pRuShThE,</t>
-  </si>
-  <si>
     <t>patir vaH</t>
   </si>
   <si>
@@ -3307,6 +3304,321 @@
   </si>
   <si>
     <t>retains 's'</t>
+  </si>
+  <si>
+    <t>1.2.10.1</t>
+  </si>
+  <si>
+    <t>3.2.8.1</t>
+  </si>
+  <si>
+    <t>6.2.1.3</t>
+  </si>
+  <si>
+    <t>1.4.13.1</t>
+  </si>
+  <si>
+    <t>4.7.14</t>
+  </si>
+  <si>
+    <t>4.3.11.1</t>
+  </si>
+  <si>
+    <t>1.5.5.1</t>
+  </si>
+  <si>
+    <t>1.5.7.1</t>
+  </si>
+  <si>
+    <t>1.5.11.4</t>
+  </si>
+  <si>
+    <t>4.1.11.1</t>
+  </si>
+  <si>
+    <t>1.2.4.1</t>
+  </si>
+  <si>
+    <t>4.6.7.5</t>
+  </si>
+  <si>
+    <t>6.1.7.2</t>
+  </si>
+  <si>
+    <t>3.2?</t>
+  </si>
+  <si>
+    <t>1.5.10.1</t>
+  </si>
+  <si>
+    <t>1.6.2.2</t>
+  </si>
+  <si>
+    <t>2.2.3.3</t>
+  </si>
+  <si>
+    <t>2.2.3.4</t>
+  </si>
+  <si>
+    <t>2.2.4.4</t>
+  </si>
+  <si>
+    <t>2.2.9.3</t>
+  </si>
+  <si>
+    <t>2.3.3.3</t>
+  </si>
+  <si>
+    <t>3.2.11.1</t>
+  </si>
+  <si>
+    <t>4.1.3.4</t>
+  </si>
+  <si>
+    <t>4.1.3.1</t>
+  </si>
+  <si>
+    <t>1.4.45.3</t>
+  </si>
+  <si>
+    <t>4.6.7.3</t>
+  </si>
+  <si>
+    <t>4.4.3.3</t>
+  </si>
+  <si>
+    <t>5.5.7.3</t>
+  </si>
+  <si>
+    <t>5.5.7.4</t>
+  </si>
+  <si>
+    <t>7.4.17.1</t>
+  </si>
+  <si>
+    <t>7.4.20.1</t>
+  </si>
+  <si>
+    <t>1.2.3.3</t>
+  </si>
+  <si>
+    <t>1.3.13.2</t>
+  </si>
+  <si>
+    <t>6.1.4.9</t>
+  </si>
+  <si>
+    <t>6.4.3.3</t>
+  </si>
+  <si>
+    <t>1.2.1.1</t>
+  </si>
+  <si>
+    <t>3.1.9.2</t>
+  </si>
+  <si>
+    <t>1.4.43.1</t>
+  </si>
+  <si>
+    <t>3.1.4.1</t>
+  </si>
+  <si>
+    <t>4.2.2.3</t>
+  </si>
+  <si>
+    <t>4.3.13.5</t>
+  </si>
+  <si>
+    <t>4.4.4.7</t>
+  </si>
+  <si>
+    <t>2.2.12.5</t>
+  </si>
+  <si>
+    <t>1.4.4.1</t>
+  </si>
+  <si>
+    <t>3.4.2.1</t>
+  </si>
+  <si>
+    <t>1.2.6.1</t>
+  </si>
+  <si>
+    <t>1.2.11.2</t>
+  </si>
+  <si>
+    <t>1.2.14.5</t>
+  </si>
+  <si>
+    <t>1.2.14.6</t>
+  </si>
+  <si>
+    <t>1.4.43.2</t>
+  </si>
+  <si>
+    <t>1.5.2.4</t>
+  </si>
+  <si>
+    <t>1.5.3.2</t>
+  </si>
+  <si>
+    <t>1.5.4.3</t>
+  </si>
+  <si>
+    <t>1.6.6.2</t>
+  </si>
+  <si>
+    <t>1.7.6.4</t>
+  </si>
+  <si>
+    <t>3.2.11.2</t>
+  </si>
+  <si>
+    <t>3.4.10.5</t>
+  </si>
+  <si>
+    <t>3.5.3.2</t>
+  </si>
+  <si>
+    <t>4.1.7.1</t>
+  </si>
+  <si>
+    <t>4.2.2.1</t>
+  </si>
+  <si>
+    <t>4.2.9.4</t>
+  </si>
+  <si>
+    <t>4.3.13.1</t>
+  </si>
+  <si>
+    <t>4.4.4.6</t>
+  </si>
+  <si>
+    <t>4.6.5.5</t>
+  </si>
+  <si>
+    <t>5.4.7.5</t>
+  </si>
+  <si>
+    <t>5.7.4.1</t>
+  </si>
+  <si>
+    <t>5.7.6.3</t>
+  </si>
+  <si>
+    <t>5.7.8.1</t>
+  </si>
+  <si>
+    <t>6.2.2.7</t>
+  </si>
+  <si>
+    <t>6.6.1.2</t>
+  </si>
+  <si>
+    <t>1.6.2.1</t>
+  </si>
+  <si>
+    <t>1.6.10.2</t>
+  </si>
+  <si>
+    <t>4.4.11.3</t>
+  </si>
+  <si>
+    <t>4.4.11.4</t>
+  </si>
+  <si>
+    <t>5.4.2.4</t>
+  </si>
+  <si>
+    <t>3.2.5.4</t>
+  </si>
+  <si>
+    <t>4.7.6.2</t>
+  </si>
+  <si>
+    <t>4.7.7.1</t>
+  </si>
+  <si>
+    <t>1.5.10.3</t>
+  </si>
+  <si>
+    <t>6.6.7.2</t>
+  </si>
+  <si>
+    <t>1.2.3.1</t>
+  </si>
+  <si>
+    <t>6.1.4.4</t>
+  </si>
+  <si>
+    <t>1.3.4.1</t>
+  </si>
+  <si>
+    <t>1.4.46.3</t>
+  </si>
+  <si>
+    <t>1.5.5.3</t>
+  </si>
+  <si>
+    <t>1.4.24.1</t>
+  </si>
+  <si>
+    <t>4.6.6.4</t>
+  </si>
+  <si>
+    <t>1.5.6.3</t>
+  </si>
+  <si>
+    <t>3.1.10.3</t>
+  </si>
+  <si>
+    <t>4.4.4.8</t>
+  </si>
+  <si>
+    <t>4.1.7.2</t>
+  </si>
+  <si>
+    <t>7.5.7.4</t>
+  </si>
+  <si>
+    <t>1.3.14.2</t>
+  </si>
+  <si>
+    <t>3.3.11.3</t>
+  </si>
+  <si>
+    <t>3.3.11.5</t>
+  </si>
+  <si>
+    <t>4.3.13.3</t>
+  </si>
+  <si>
+    <t>4.7.15.5</t>
+  </si>
+  <si>
+    <t>7.5.24.1</t>
+  </si>
+  <si>
+    <t>1.8.12.2</t>
+  </si>
+  <si>
+    <t>3.2.4.1</t>
+  </si>
+  <si>
+    <t>pRuShThE</t>
+  </si>
+  <si>
+    <t>4.2.7.2</t>
+  </si>
+  <si>
+    <t>asME</t>
+  </si>
+  <si>
+    <t>amartya</t>
+  </si>
+  <si>
+    <t>No elision</t>
   </si>
 </sst>
 </file>
@@ -3430,7 +3742,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3467,6 +3779,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3495,7 +3819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3564,6 +3888,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4472,7 +4801,7 @@
         <v>10</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
@@ -5435,7 +5764,7 @@
         <v>9</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D90" s="15"/>
       <c r="E90" s="15"/>
@@ -5454,7 +5783,7 @@
         <v>10</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D91" s="15"/>
       <c r="E91" s="15"/>
@@ -5855,7 +6184,7 @@
         <v>109</v>
       </c>
       <c r="D112" s="21" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E112" s="15" t="s">
         <v>110</v>
@@ -6365,7 +6694,7 @@
         <v>26</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="15"/>
@@ -6402,7 +6731,7 @@
         <v>136</v>
       </c>
       <c r="D141" s="24" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E141" s="15" t="s">
         <v>137</v>
@@ -6456,7 +6785,7 @@
         <v>2</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="15"/>
@@ -6885,7 +7214,7 @@
     <row r="167" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A167" s="15"/>
       <c r="B167" s="15">
-        <f t="shared" ref="B167:B170" si="6">+B166+1</f>
+        <f>+B166+1</f>
         <v>2</v>
       </c>
       <c r="C167" s="15" t="s">
@@ -6904,7 +7233,7 @@
     <row r="168" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A168" s="15"/>
       <c r="B168" s="15">
-        <f t="shared" si="6"/>
+        <f>+B167+1</f>
         <v>3</v>
       </c>
       <c r="C168" s="15" t="s">
@@ -6923,7 +7252,7 @@
     <row r="169" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A169" s="15"/>
       <c r="B169" s="15">
-        <f t="shared" si="6"/>
+        <f>+B168+1</f>
         <v>4</v>
       </c>
       <c r="C169" s="15" t="s">
@@ -6942,7 +7271,7 @@
     <row r="170" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A170" s="15"/>
       <c r="B170" s="15">
-        <f t="shared" si="6"/>
+        <f>+B169+1</f>
         <v>5</v>
       </c>
       <c r="C170" s="15" t="s">
@@ -6995,7 +7324,7 @@
     <row r="173" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A173" s="15"/>
       <c r="B173" s="15">
-        <f t="shared" ref="B173:B177" si="7">+B172+1</f>
+        <f>+B172+1</f>
         <v>2</v>
       </c>
       <c r="C173" s="15" t="s">
@@ -7014,7 +7343,7 @@
     <row r="174" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A174" s="15"/>
       <c r="B174" s="15">
-        <f t="shared" si="7"/>
+        <f>+B173+1</f>
         <v>3</v>
       </c>
       <c r="C174" s="15" t="s">
@@ -7033,7 +7362,7 @@
     <row r="175" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A175" s="15"/>
       <c r="B175" s="15">
-        <f t="shared" si="7"/>
+        <f>+B174+1</f>
         <v>4</v>
       </c>
       <c r="C175" s="15" t="s">
@@ -7052,7 +7381,7 @@
     <row r="176" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A176" s="15"/>
       <c r="B176" s="15">
-        <f t="shared" si="7"/>
+        <f>+B175+1</f>
         <v>5</v>
       </c>
       <c r="C176" s="15" t="s">
@@ -7071,7 +7400,7 @@
     <row r="177" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A177" s="15"/>
       <c r="B177" s="15">
-        <f t="shared" si="7"/>
+        <f>+B176+1</f>
         <v>6</v>
       </c>
       <c r="C177" s="15" t="s">
@@ -7250,10 +7579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L218"/>
+  <dimension ref="A2:N218"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I98" sqref="I98"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7264,13 +7593,13 @@
     <col min="10" max="10" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>173</v>
       </c>
@@ -7281,7 +7610,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="25" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="25" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B4" s="25" t="s">
         <v>175</v>
       </c>
@@ -7292,7 +7621,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C5" s="25">
         <v>4.2</v>
       </c>
@@ -7308,7 +7637,7 @@
       <c r="K5" s="25"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C6" s="25">
         <v>4.3</v>
       </c>
@@ -7324,7 +7653,7 @@
       <c r="K6" s="25"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C7" s="25">
         <v>4.4000000000000004</v>
       </c>
@@ -7340,7 +7669,7 @@
       <c r="K7" s="25"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="25">
         <v>4.5</v>
       </c>
@@ -7356,7 +7685,7 @@
       <c r="K8" s="25"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="25">
         <v>4.5999999999999996</v>
       </c>
@@ -7372,7 +7701,7 @@
       <c r="K9" s="25"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="25"/>
       <c r="D10" s="25" t="s">
         <v>184</v>
@@ -7386,7 +7715,7 @@
       <c r="K10" s="25"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C11" s="25">
         <v>4.7</v>
       </c>
@@ -7402,7 +7731,7 @@
       <c r="K11" s="25"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="C12" s="25">
         <v>4.8</v>
       </c>
@@ -7418,7 +7747,7 @@
       <c r="K12" s="25"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="14" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>4.9000000000000004</v>
       </c>
@@ -7426,8 +7755,23 @@
       <c r="C14" s="15" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="J14" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="37">
         <v>4.0999999999999996</v>
       </c>
@@ -7438,7 +7782,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="36">
         <v>4.1100000000000003</v>
       </c>
@@ -7689,7 +8033,7 @@
         <v>28</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="44" spans="2:3" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7725,7 +8069,7 @@
         <v>32</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="48" spans="2:3" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7770,7 +8114,7 @@
         <v>4.12</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>235</v>
@@ -7826,7 +8170,7 @@
     </row>
     <row r="60" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C60" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>234</v>
@@ -7834,7 +8178,7 @@
     </row>
     <row r="61" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C61" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>234</v>
@@ -7858,7 +8202,7 @@
     </row>
     <row r="64" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C64" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>234</v>
@@ -7902,7 +8246,7 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>241</v>
@@ -7970,7 +8314,7 @@
     </row>
     <row r="79" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C79" s="4" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>244</v>
@@ -8111,7 +8455,7 @@
         <v>262</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="98" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8119,7 +8463,7 @@
         <v>4.25</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>268</v>
@@ -8495,7 +8839,7 @@
         <v>308</v>
       </c>
       <c r="I128" s="4" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="129" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8763,7 +9107,7 @@
     <row r="153" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="154" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B154" s="34" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C154" s="34"/>
       <c r="D154" s="34"/>
@@ -8831,7 +9175,7 @@
     </row>
     <row r="163" spans="1:4" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B163" s="4">
-        <f t="shared" ref="B163:B166" si="2">+B162+1</f>
+        <f>+B162+1</f>
         <v>3</v>
       </c>
       <c r="C163" s="4" t="s">
@@ -8840,7 +9184,7 @@
     </row>
     <row r="164" spans="1:4" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B164" s="4">
-        <f t="shared" si="2"/>
+        <f>+B163+1</f>
         <v>4</v>
       </c>
       <c r="C164" s="4" t="s">
@@ -8849,7 +9193,7 @@
     </row>
     <row r="165" spans="1:4" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B165" s="4">
-        <f t="shared" si="2"/>
+        <f>+B164+1</f>
         <v>5</v>
       </c>
       <c r="C165" s="4" t="s">
@@ -8858,7 +9202,7 @@
     </row>
     <row r="166" spans="1:4" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B166" s="4">
-        <f t="shared" si="2"/>
+        <f>+B165+1</f>
         <v>6</v>
       </c>
       <c r="C166" s="4" t="s">
@@ -8948,7 +9292,7 @@
   <dimension ref="A2:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
@@ -9268,7 +9612,7 @@
         <v>380</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>377</v>
@@ -9282,7 +9626,7 @@
         <v>381</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>377</v>
@@ -9296,7 +9640,7 @@
         <v>382</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>377</v>
@@ -9418,13 +9762,13 @@
         <v>279</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="J33" s="4" t="s">
         <v>1021</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9438,7 +9782,7 @@
         <v>279</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9452,10 +9796,10 @@
         <v>279</v>
       </c>
       <c r="H35" s="4" t="s">
+        <v>1023</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>1024</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9469,7 +9813,7 @@
         <v>279</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9483,12 +9827,12 @@
         <v>279</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C38" s="4" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>400</v>
@@ -9497,7 +9841,7 @@
         <v>279</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9541,10 +9885,10 @@
   <dimension ref="A2:Q104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9605,7 +9949,7 @@
         <v>370</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9619,7 +9963,7 @@
         <v>370</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9633,7 +9977,7 @@
         <v>370</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9647,7 +9991,7 @@
         <v>370</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9696,7 +10040,7 @@
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>356</v>
@@ -9705,7 +10049,7 @@
         <v>370</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9719,7 +10063,7 @@
         <v>370</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9733,7 +10077,7 @@
         <v>370</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9750,7 +10094,7 @@
         <v>417</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9758,7 +10102,7 @@
         <v>418</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -9767,7 +10111,7 @@
         <v>6.4</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -10115,7 +10459,7 @@
         <v>6.9</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E66" s="41"/>
     </row>
@@ -10153,7 +10497,7 @@
         <v>448</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10161,7 +10505,7 @@
         <v>449</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="74" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10169,7 +10513,7 @@
         <v>450</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10177,7 +10521,7 @@
         <v>445</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10185,7 +10529,7 @@
         <v>451</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="77" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10193,7 +10537,7 @@
         <v>452</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10201,7 +10545,7 @@
         <v>453</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="79" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10209,7 +10553,7 @@
         <v>454</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="80" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10217,7 +10561,7 @@
         <v>455</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="81" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10225,7 +10569,7 @@
         <v>456</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="82" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10233,7 +10577,7 @@
         <v>457</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="83" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10241,7 +10585,7 @@
         <v>458</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="84" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10249,7 +10593,7 @@
         <v>459</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="85" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -10264,16 +10608,16 @@
         <v>414</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>484</v>
       </c>
       <c r="K86" s="4" t="s">
+        <v>981</v>
+      </c>
+      <c r="L86" s="4" t="s">
         <v>982</v>
-      </c>
-      <c r="L86" s="4" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="87" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10284,13 +10628,13 @@
         <v>414</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H87" s="4" t="s">
+        <v>983</v>
+      </c>
+      <c r="I87" s="4" t="s">
         <v>984</v>
-      </c>
-      <c r="I87" s="4" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="88" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10301,10 +10645,10 @@
         <v>414</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="89" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10315,31 +10659,31 @@
         <v>414</v>
       </c>
       <c r="F89" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="H89" s="4" t="s">
         <v>965</v>
       </c>
-      <c r="H89" s="4" t="s">
-        <v>966</v>
-      </c>
       <c r="I89" s="4" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="L89" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="M89" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="N89" s="4" t="s">
         <v>999</v>
       </c>
-      <c r="M89" s="4" t="s">
-        <v>998</v>
-      </c>
-      <c r="N89" s="4" t="s">
+      <c r="O89" s="4" t="s">
         <v>1000</v>
       </c>
-      <c r="O89" s="4" t="s">
+      <c r="P89" s="4" t="s">
         <v>1001</v>
       </c>
-      <c r="P89" s="4" t="s">
+      <c r="Q89" s="4" t="s">
         <v>1002</v>
-      </c>
-      <c r="Q89" s="4" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="90" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10350,25 +10694,25 @@
         <v>414</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H90" s="4" t="s">
+        <v>967</v>
+      </c>
+      <c r="I90" s="4" t="s">
         <v>968</v>
       </c>
-      <c r="I90" s="4" t="s">
+      <c r="J90" s="4" t="s">
         <v>969</v>
       </c>
-      <c r="J90" s="4" t="s">
+      <c r="K90" s="4" t="s">
         <v>970</v>
       </c>
-      <c r="K90" s="4" t="s">
+      <c r="L90" s="4" t="s">
         <v>971</v>
       </c>
-      <c r="L90" s="4" t="s">
-        <v>972</v>
-      </c>
       <c r="M90" s="4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10380,10 +10724,10 @@
         <v>414</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10395,28 +10739,28 @@
         <v>414</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C93" s="5" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
         <v>414</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10428,31 +10772,31 @@
         <v>414</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C95" s="4" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
         <v>414</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="K95" s="4" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10464,28 +10808,28 @@
         <v>414</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I96" s="4" t="s">
+        <v>991</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="K96" s="4" t="s">
         <v>992</v>
       </c>
-      <c r="J96" s="4" t="s">
-        <v>847</v>
-      </c>
-      <c r="K96" s="4" t="s">
+      <c r="L96" s="4" t="s">
         <v>993</v>
       </c>
-      <c r="L96" s="4" t="s">
+      <c r="M96" s="4" t="s">
         <v>994</v>
       </c>
-      <c r="M96" s="4" t="s">
+      <c r="N96" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="N96" s="4" t="s">
-        <v>996</v>
-      </c>
       <c r="O96" s="4" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="97" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10497,10 +10841,10 @@
         <v>414</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="98" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10512,10 +10856,10 @@
         <v>414</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="99" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10527,10 +10871,10 @@
         <v>414</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="100" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10542,10 +10886,10 @@
         <v>414</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="101" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10557,10 +10901,10 @@
         <v>414</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="102" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10570,7 +10914,7 @@
     </row>
     <row r="103" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C103" s="25" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -10592,10 +10936,10 @@
   <dimension ref="A3:L294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10636,7 +10980,7 @@
         <v>7.2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>279</v>
@@ -10647,7 +10991,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>279</v>
@@ -10667,7 +11011,7 @@
         <v>402</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10681,7 +11025,7 @@
         <v>402</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10695,7 +11039,7 @@
         <v>402</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10709,13 +11053,13 @@
         <v>402</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>960</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>961</v>
-      </c>
       <c r="I12" s="4" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10729,7 +11073,7 @@
         <v>402</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10754,7 +11098,7 @@
         <v>402</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10793,7 +11137,7 @@
         <v>495</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -10849,10 +11193,10 @@
         <v>498</v>
       </c>
       <c r="G28" s="4" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>1014</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10860,13 +11204,13 @@
         <v>499</v>
       </c>
       <c r="G29" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>1016</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>1015</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>1017</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>443</v>
@@ -10877,7 +11221,7 @@
         <v>500</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10915,10 +11259,10 @@
         <v>505</v>
       </c>
       <c r="F36" s="4" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>1007</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10929,10 +11273,10 @@
         <v>506</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -10947,10 +11291,10 @@
         <v>507</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10961,10 +11305,10 @@
         <v>509</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -11274,7 +11618,7 @@
         <v>620</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>624</v>
@@ -11288,7 +11632,7 @@
         <v>621</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>624</v>
@@ -11302,7 +11646,7 @@
         <v>622</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>624</v>
@@ -11316,7 +11660,7 @@
         <v>623</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>624</v>
@@ -11337,7 +11681,7 @@
         <v>632</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11348,7 +11692,7 @@
         <v>632</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11359,7 +11703,7 @@
         <v>632</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11370,7 +11714,7 @@
         <v>632</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11381,7 +11725,7 @@
         <v>632</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11392,7 +11736,7 @@
         <v>632</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="93" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -11401,7 +11745,7 @@
         <v>633</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11409,7 +11753,7 @@
         <v>634</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11417,7 +11761,7 @@
         <v>635</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11425,7 +11769,7 @@
         <v>636</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="98" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11433,7 +11777,7 @@
         <v>637</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11441,7 +11785,7 @@
         <v>638</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11449,7 +11793,7 @@
         <v>639</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="101" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11457,7 +11801,7 @@
         <v>640</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="102" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11465,7 +11809,7 @@
         <v>641</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="103" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11473,7 +11817,7 @@
         <v>642</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11481,7 +11825,7 @@
         <v>643</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -11490,7 +11834,7 @@
         <v>9.2200000000000006</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>644</v>
@@ -11499,15 +11843,15 @@
         <v>279</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>542</v>
@@ -11516,12 +11860,12 @@
         <v>279</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="108" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B108" s="4" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>645</v>
@@ -11530,12 +11874,12 @@
         <v>279</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B109" s="4" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>646</v>
@@ -11544,15 +11888,15 @@
         <v>279</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
+        <v>934</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>935</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>936</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>647</v>
@@ -11561,12 +11905,12 @@
         <v>279</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B111" s="4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>648</v>
@@ -11575,7 +11919,7 @@
         <v>279</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11586,15 +11930,15 @@
         <v>279</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="113" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>650</v>
@@ -11603,15 +11947,15 @@
         <v>279</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="114" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="B114" s="4" t="s">
         <v>937</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>938</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>651</v>
@@ -11620,15 +11964,15 @@
         <v>279</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="115" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
+        <v>938</v>
+      </c>
+      <c r="B115" s="4" t="s">
         <v>939</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>940</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>439</v>
@@ -11637,27 +11981,27 @@
         <v>279</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G115" s="4" t="s">
+        <v>940</v>
+      </c>
+      <c r="H115" s="4" t="s">
         <v>941</v>
       </c>
-      <c r="H115" s="4" t="s">
+      <c r="I115" s="4" t="s">
         <v>942</v>
       </c>
-      <c r="I115" s="4" t="s">
+      <c r="J115" s="4" t="s">
         <v>943</v>
       </c>
-      <c r="J115" s="4" t="s">
+      <c r="K115" s="4" t="s">
         <v>944</v>
-      </c>
-      <c r="K115" s="4" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="116" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>652</v>
@@ -11666,12 +12010,12 @@
         <v>279</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="117" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>653</v>
@@ -11680,15 +12024,15 @@
         <v>279</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="118" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>948</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>949</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>654</v>
@@ -11697,12 +12041,12 @@
         <v>279</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="119" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>655</v>
@@ -11711,23 +12055,23 @@
         <v>279</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="120" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C120" s="5" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>279</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="121" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>656</v>
@@ -11736,24 +12080,24 @@
         <v>279</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="I121" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="J121" s="4" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K121" s="4" t="s">
         <v>1004</v>
       </c>
-      <c r="K121" s="4" t="s">
-        <v>1005</v>
-      </c>
       <c r="L121" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="122" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>657</v>
@@ -11762,7 +12106,7 @@
         <v>279</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="123" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -11889,7 +12233,7 @@
     </row>
     <row r="136" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E136" s="4" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F136" s="4" t="s">
         <v>402</v>
@@ -11916,40 +12260,40 @@
         <v>13.5</v>
       </c>
       <c r="C139" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="G139" s="4" t="s">
         <v>889</v>
-      </c>
-      <c r="G139" s="4" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="140" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G140" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="141" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G141" s="4" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="142" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G142" s="4" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="143" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G143" s="4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="144" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G144" s="4" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="145" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G145" s="4" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="146" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12885,7 +13229,7 @@
     <row r="86" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C87" s="38" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12896,7 +13240,7 @@
         <v>605</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12904,7 +13248,7 @@
         <v>563</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12912,7 +13256,7 @@
         <v>606</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12920,7 +13264,7 @@
         <v>607</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12928,7 +13272,7 @@
         <v>544</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13024,13 +13368,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G201"/>
+  <dimension ref="A2:P203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C114" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D67" sqref="D67"/>
+      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13181,7 +13525,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>12.5</v>
       </c>
@@ -13195,7 +13539,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C18" s="29" t="s">
         <v>686</v>
       </c>
@@ -13206,8 +13550,8 @@
         <v>618</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="29">
         <v>12.6</v>
       </c>
@@ -13217,23 +13561,56 @@
       <c r="D20" s="4" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H20" s="44" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I20" s="45" t="s">
+        <v>1052</v>
+      </c>
+      <c r="J20" s="44" t="s">
+        <v>1053</v>
+      </c>
+      <c r="K20" s="44" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L20" s="44" t="s">
+        <v>1055</v>
+      </c>
+      <c r="M20" s="44" t="s">
+        <v>1056</v>
+      </c>
+      <c r="N20" s="44" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H21" s="44" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H22" s="44" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D23" s="4" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H23" s="44" t="s">
+        <v>1060</v>
+      </c>
+      <c r="I23" s="44" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="29">
         <v>12.7</v>
       </c>
@@ -13247,7 +13624,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E25" s="4" t="s">
         <v>692</v>
       </c>
@@ -13255,7 +13632,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E26" s="4" t="s">
         <v>693</v>
       </c>
@@ -13263,15 +13640,15 @@
         <v>618</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E27" s="4" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G27" s="29" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E28" s="4" t="s">
         <v>694</v>
       </c>
@@ -13279,7 +13656,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E29" s="4" t="s">
         <v>695</v>
       </c>
@@ -13287,7 +13664,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E30" s="4" t="s">
         <v>696</v>
       </c>
@@ -13295,7 +13672,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E31" s="4" t="s">
         <v>697</v>
       </c>
@@ -13303,7 +13680,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E32" s="4" t="s">
         <v>698</v>
       </c>
@@ -13570,7 +13947,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
         <v>730</v>
       </c>
@@ -13578,15 +13955,15 @@
         <v>618</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="G66" s="29" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D67" s="4" t="s">
         <v>731</v>
       </c>
@@ -13594,8 +13971,8 @@
         <v>618</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>734</v>
       </c>
@@ -13604,8 +13981,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="29">
         <v>11.3</v>
       </c>
@@ -13615,16 +13992,25 @@
       <c r="F71" s="29" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H71" s="29" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C72" s="29" t="s">
         <v>735</v>
       </c>
       <c r="F72" s="29" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H72" s="29">
+        <v>5.6</v>
+      </c>
+      <c r="I72" s="29">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C73" s="29" t="s">
         <v>737</v>
       </c>
@@ -13632,55 +14018,97 @@
         <v>738</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C74" s="29" t="s">
         <v>739</v>
       </c>
       <c r="F74" s="29" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H74" s="42" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I74" s="42" t="s">
+        <v>935</v>
+      </c>
+      <c r="J74" s="42" t="s">
+        <v>1048</v>
+      </c>
+      <c r="K74" s="42" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C75" s="29" t="s">
         <v>739</v>
       </c>
       <c r="F75" s="29" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H75" s="42" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I75" s="44" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J75" s="42" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C76" s="29" t="s">
         <v>742</v>
       </c>
       <c r="F76" s="29" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H76" s="29">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C77" s="29" t="s">
         <v>739</v>
       </c>
       <c r="F77" s="29" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H77" s="42" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C78" s="29" t="s">
         <v>739</v>
       </c>
       <c r="F78" s="29" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H78" s="44" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C79" s="29" t="s">
         <v>739</v>
       </c>
       <c r="F79" s="29" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H79" s="44" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I79" s="42" t="s">
+        <v>1044</v>
+      </c>
+      <c r="J79" s="43" t="s">
+        <v>1045</v>
+      </c>
+      <c r="K79" s="43" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C80" s="29" t="s">
         <v>747</v>
       </c>
@@ -13688,7 +14116,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C81" s="29" t="s">
         <v>737</v>
       </c>
@@ -13696,23 +14124,29 @@
         <v>749</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C82" s="29" t="s">
         <v>737</v>
       </c>
       <c r="F82" s="4" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="I82" s="29" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C83" s="29" t="s">
         <v>737</v>
       </c>
       <c r="F83" s="4" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H83" s="29" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C84" s="29" t="s">
         <v>737</v>
       </c>
@@ -13720,7 +14154,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C85" s="29" t="s">
         <v>737</v>
       </c>
@@ -13728,8 +14162,8 @@
         <v>751</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A87" s="29">
         <v>11.4</v>
       </c>
@@ -13737,32 +14171,32 @@
         <v>759</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E88" s="4" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E89" s="4" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E90" s="4" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E91" s="4" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E92" s="4" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="29">
         <v>11.5</v>
       </c>
@@ -13772,57 +14206,96 @@
       <c r="D93" s="4" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="G93" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H93" s="45" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="C94" s="4" t="s">
         <v>765</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H94" s="45" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C95" s="4" t="s">
         <v>762</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G95" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H95" s="45" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C96" s="4" t="s">
         <v>763</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C97" s="4" t="s">
-        <v>912</v>
-      </c>
-      <c r="D97" s="4" t="s">
+      <c r="G96" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H96" s="45" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C97" s="6" t="s">
+        <v>911</v>
+      </c>
+      <c r="D97" s="6" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="98" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C98" s="4" t="s">
         <v>764</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G98" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H98" s="45" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C99" s="4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G99" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H99" s="45" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I99" s="45" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J99" s="45" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A101" s="29">
         <v>11.6</v>
       </c>
@@ -13832,17 +14305,29 @@
       <c r="D101" s="4" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G101" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H101" s="45" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C102" s="4" t="s">
         <v>766</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G102" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H102" s="45" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="29">
         <v>11.7</v>
       </c>
@@ -13852,48 +14337,81 @@
       <c r="D104" s="4" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G104" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H104" s="45" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C105" s="4" t="s">
         <v>768</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G105" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H105" s="45" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
     </row>
-    <row r="107" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="29">
         <v>11.8</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="6" t="s">
         <v>770</v>
       </c>
     </row>
-    <row r="108" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C108" s="4" t="s">
         <v>265</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G108" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H108" s="45" t="s">
+        <v>1068</v>
+      </c>
+      <c r="I108" s="45" t="s">
+        <v>1069</v>
+      </c>
+      <c r="J108" s="45" t="s">
+        <v>1070</v>
+      </c>
+      <c r="K108" s="45" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C109" s="4" t="s">
         <v>265</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G109" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H109" s="45" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A111" s="29">
         <v>11.9</v>
       </c>
@@ -13903,8 +14421,14 @@
       <c r="D111" s="4" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G111" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H111" s="45" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C112" s="4" t="s">
         <v>381</v>
       </c>
@@ -13912,23 +14436,29 @@
         <v>774</v>
       </c>
     </row>
-    <row r="113" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C113" s="3" t="s">
         <v>505</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="G113" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="H113" s="45" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
     </row>
-    <row r="115" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="1:4" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:16" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A116" s="31">
         <v>11.1</v>
       </c>
@@ -13938,459 +14468,670 @@
       <c r="D116" s="4" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H116" s="44" t="s">
+        <v>1079</v>
+      </c>
+      <c r="I116" s="44" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J116" s="44" t="s">
+        <v>1076</v>
+      </c>
+      <c r="K116" s="44" t="s">
+        <v>1077</v>
+      </c>
+      <c r="L116" s="44" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C117" s="4" t="s">
         <v>775</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H117" s="44" t="s">
+        <v>1080</v>
+      </c>
+      <c r="I117" s="44" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C118" s="4" t="s">
         <v>775</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H118" s="44" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C119" s="4" t="s">
         <v>775</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A121" s="29">
+      <c r="H119" s="44" t="s">
+        <v>1083</v>
+      </c>
+      <c r="I119" s="44" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J119" s="44" t="s">
+        <v>1085</v>
+      </c>
+      <c r="K119" s="44" t="s">
+        <v>1086</v>
+      </c>
+      <c r="L119" s="44" t="s">
+        <v>1087</v>
+      </c>
+      <c r="M119" s="44" t="s">
+        <v>1088</v>
+      </c>
+      <c r="N119" s="44" t="s">
+        <v>1089</v>
+      </c>
+      <c r="O119" s="44" t="s">
+        <v>1090</v>
+      </c>
+      <c r="P119" s="44" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H120" s="44" t="s">
+        <v>1030</v>
+      </c>
+      <c r="I120" s="44" t="s">
+        <v>1092</v>
+      </c>
+      <c r="J120" s="44" t="s">
+        <v>1093</v>
+      </c>
+      <c r="K120" s="44" t="s">
+        <v>1094</v>
+      </c>
+      <c r="L120" s="44" t="s">
+        <v>1095</v>
+      </c>
+      <c r="M120" s="44" t="s">
+        <v>967</v>
+      </c>
+      <c r="N120" s="44" t="s">
+        <v>1096</v>
+      </c>
+      <c r="O120" s="44" t="s">
+        <v>1097</v>
+      </c>
+      <c r="P120" s="44" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H121" s="44" t="s">
+        <v>1099</v>
+      </c>
+      <c r="I121" s="44" t="s">
+        <v>1100</v>
+      </c>
+      <c r="J121" s="44" t="s">
+        <v>1101</v>
+      </c>
+      <c r="K121" s="44" t="s">
+        <v>1102</v>
+      </c>
+      <c r="L121" s="44" t="s">
+        <v>1103</v>
+      </c>
+      <c r="M121" s="44" t="s">
+        <v>1104</v>
+      </c>
+      <c r="N121" s="44" t="s">
+        <v>1105</v>
+      </c>
+      <c r="O121" s="44" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A123" s="29">
         <v>11.11</v>
       </c>
-      <c r="C121" s="4" t="s">
-        <v>780</v>
-      </c>
-      <c r="D121" s="4" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A122" s="29">
-        <v>11.12</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>780</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C123" s="4" t="s">
         <v>780</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>779</v>
+      </c>
+      <c r="H123" s="44" t="s">
+        <v>1107</v>
+      </c>
+      <c r="I123" s="44" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J123" s="44" t="s">
+        <v>1109</v>
+      </c>
+      <c r="K123" s="44" t="s">
+        <v>1110</v>
+      </c>
+      <c r="L123" s="44" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A124" s="29">
+        <v>11.12</v>
+      </c>
       <c r="C124" s="4" t="s">
         <v>780</v>
       </c>
       <c r="D124" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="H124" s="44" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C125" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="H125" s="44" t="s">
+        <v>1112</v>
+      </c>
+      <c r="I125" s="43" t="s">
+        <v>1113</v>
+      </c>
+      <c r="J125" s="43" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C126" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="D126" s="4" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A126" s="29">
+      <c r="H126" s="44" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A128" s="29">
         <v>11.13</v>
       </c>
-      <c r="C126" s="4" t="s">
-        <v>784</v>
-      </c>
-      <c r="D126" s="4" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C127" s="4" t="s">
-        <v>784</v>
-      </c>
-      <c r="D127" s="4" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C128" s="4" t="s">
         <v>784</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>785</v>
+      </c>
+      <c r="H128" s="44" t="s">
+        <v>1117</v>
+      </c>
+      <c r="I128" s="44" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C129" s="4" t="s">
         <v>784</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+      <c r="H129" s="44" t="s">
+        <v>1119</v>
+      </c>
+      <c r="I129" s="43" t="s">
+        <v>930</v>
+      </c>
+      <c r="J129" s="44" t="s">
+        <v>956</v>
+      </c>
+      <c r="K129" s="44" t="s">
+        <v>1120</v>
+      </c>
+      <c r="L129" s="43" t="s">
+        <v>1121</v>
+      </c>
+      <c r="M129" s="29" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C130" s="4" t="s">
         <v>784</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>786</v>
+      </c>
+      <c r="H130" s="44" t="s">
+        <v>1122</v>
+      </c>
+      <c r="I130" s="44" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C131" s="4" t="s">
         <v>784</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>787</v>
+      </c>
+      <c r="H131" s="44" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I131" s="44" t="s">
+        <v>1125</v>
+      </c>
+      <c r="J131" s="44" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C132" s="4" t="s">
         <v>784</v>
       </c>
       <c r="D132" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="H132" s="44" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I132" s="44" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C133" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="H133" s="44" t="s">
+        <v>958</v>
+      </c>
+      <c r="I133" s="44" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C134" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="D134" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A134" s="29">
+      <c r="H134" s="46" t="s">
+        <v>1129</v>
+      </c>
+      <c r="I134" s="46" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J134" s="46" t="s">
+        <v>1131</v>
+      </c>
+      <c r="K134" s="46" t="s">
+        <v>1132</v>
+      </c>
+      <c r="L134" s="43" t="s">
+        <v>1133</v>
+      </c>
+      <c r="M134" s="46" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A136" s="29">
         <v>11.14</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C136" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D136" s="4" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="135" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C135" s="4"/>
-      <c r="D135" s="4" t="s">
+    <row r="137" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C137" s="4"/>
+      <c r="D137" s="4" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="136" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C136" s="4"/>
-      <c r="D136" s="4" t="s">
+    <row r="138" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C138" s="4"/>
+      <c r="D138" s="4" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="137" spans="1:4" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A138" s="29">
+    <row r="139" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A140" s="29">
         <v>11.15</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C140" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D140" s="4" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C139" s="4" t="s">
+      <c r="H140" s="44" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C141" s="4" t="s">
         <v>795</v>
       </c>
-      <c r="D139" s="4" t="s">
+      <c r="D141" s="4" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A141" s="29">
+      <c r="H141" s="44" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A143" s="29">
         <v>11.16</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D143" s="4" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="142" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D142" s="4" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D143" s="4" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D144" s="4" t="s">
-        <v>798</v>
+        <v>817</v>
       </c>
     </row>
     <row r="145" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D145" s="4" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="146" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D146" s="4" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="147" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D147" s="4" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="148" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D148" s="4" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="149" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D149" s="4" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="150" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D150" s="4" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="151" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D151" s="4" t="s">
-        <v>914</v>
+        <v>803</v>
       </c>
     </row>
     <row r="152" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D152" s="4" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="153" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D153" s="4" t="s">
-        <v>806</v>
+        <v>913</v>
       </c>
     </row>
     <row r="154" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D154" s="4" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="155" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D155" s="4" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="156" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D156" s="4" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="157" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D157" s="4" t="s">
-        <v>810</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="158" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D158" s="4" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="159" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D159" s="4" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
     </row>
     <row r="160" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D160" s="4" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="161" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D161" s="4" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
     </row>
     <row r="162" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D162" s="4" t="s">
-        <v>898</v>
+        <v>811</v>
       </c>
     </row>
     <row r="163" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D163" s="4" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
     </row>
     <row r="164" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D164" s="4" t="s">
-        <v>814</v>
+        <v>897</v>
       </c>
     </row>
     <row r="165" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D165" s="4" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
     </row>
     <row r="166" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D166" s="4" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D167" s="4" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D168" s="4" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D169" s="4" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D167" s="4" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A169" s="4">
+    <row r="171" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A171" s="4">
         <v>11.17</v>
       </c>
-      <c r="E169" s="4" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E170" s="4" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E171" s="4" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E172" s="4" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E173" s="4" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E174" s="4" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E175" s="4" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E176" s="4" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
     </row>
     <row r="177" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E177" s="4" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="178" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E178" s="4" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="179" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E179" s="4" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
     </row>
     <row r="180" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E180" s="4" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
     </row>
     <row r="181" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E181" s="4" t="s">
-        <v>899</v>
+        <v>830</v>
       </c>
     </row>
     <row r="182" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E182" s="4" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="183" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E183" s="4" t="s">
-        <v>834</v>
+        <v>898</v>
       </c>
     </row>
     <row r="184" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E184" s="4" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="185" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E185" s="4" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
     </row>
     <row r="186" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E186" s="4" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
     </row>
     <row r="187" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E187" s="4" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
     </row>
     <row r="188" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E188" s="4" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
     </row>
     <row r="189" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E189" s="4" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="190" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E190" s="4" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
     </row>
     <row r="191" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E191" s="4" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
     </row>
     <row r="192" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E192" s="4" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="193" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E193" s="4" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="194" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A194" s="4">
+      <c r="E194" s="4" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E195" s="4" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A196" s="4">
         <v>11.18</v>
       </c>
-      <c r="C194" s="4" t="s">
+      <c r="C196" s="4" t="s">
+        <v>844</v>
+      </c>
+      <c r="F196" s="4" t="s">
         <v>845</v>
       </c>
-      <c r="F194" s="4" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="196" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    </row>
     <row r="197" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="198" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="199" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="200" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="201" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="202" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="203" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14400,7 +15141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G113"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -14420,10 +15161,10 @@
     </row>
     <row r="3" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>848</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>849</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -14434,7 +15175,7 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>668</v>
@@ -14443,10 +15184,10 @@
         <v>346</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>850</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>851</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14454,58 +15195,58 @@
         <v>16.2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>739</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>739</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>739</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>856</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>857</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>739</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -14514,7 +15255,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -14523,10 +15264,10 @@
         <v>16.5</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>860</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14534,7 +15275,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -14543,18 +15284,18 @@
         <v>16.7</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C18" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>864</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -14563,10 +15304,10 @@
         <v>16.8</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>866</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14574,10 +15315,10 @@
         <v>16.899999999999999</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14585,10 +15326,10 @@
         <v>16.899999999999999</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14596,7 +15337,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14604,7 +15345,7 @@
         <v>16.11</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14612,34 +15353,34 @@
         <v>16.12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C26" s="4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C27" s="4" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C28" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>875</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -14648,18 +15389,18 @@
         <v>16.25</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C31" s="4" t="s">
+        <v>877</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>878</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14667,7 +15408,7 @@
         <v>492</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -14676,35 +15417,35 @@
         <v>16.27</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>883</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C35" s="4" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>883</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C36" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>882</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>883</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -14716,21 +15457,21 @@
         <v>354</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>885</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>886</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C39" s="4" t="s">
+        <v>884</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>885</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>886</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Latest files Pushed as on 24/07/2019
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -10935,11 +10935,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D108" sqref="D108"/>
+      <selection pane="bottomRight" activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12456,7 +12456,7 @@
   <dimension ref="A2:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="L100" sqref="L100"/>
@@ -13370,7 +13370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>

</xml_diff>

<commit_message>
JD JM Files plus SJ Baraha 18/01/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -9702,10 +9702,10 @@
   <dimension ref="A2:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
+      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10295,10 +10295,10 @@
   <dimension ref="A2:Q104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11345,11 +11345,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C118" sqref="C118"/>
+      <selection pane="bottomRight" activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12866,10 +12866,10 @@
   <dimension ref="A2:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13780,11 +13780,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C186" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C158" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E187" sqref="E187"/>
+      <selection pane="bottomRight" activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Jatai Ghanam work as of 23/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="1143">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -1959,9 +1959,6 @@
   </si>
   <si>
     <t>arAn</t>
-  </si>
-  <si>
-    <t>posAn</t>
   </si>
   <si>
     <t>mahAn</t>
@@ -2718,9 +2715,6 @@
     </r>
   </si>
   <si>
-    <t>addhvara</t>
-  </si>
-  <si>
     <t>when a vowel follows 'r'</t>
   </si>
   <si>
@@ -3622,6 +3616,12 @@
   </si>
   <si>
     <t>4.43 But not when unaccented, under any circumstances.</t>
+  </si>
+  <si>
+    <t>addhvaraH</t>
+  </si>
+  <si>
+    <t>poShAn</t>
   </si>
 </sst>
 </file>
@@ -3822,7 +3822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3897,6 +3897,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4179,7 +4180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L192"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A77" workbookViewId="0">
       <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
@@ -4805,7 +4806,7 @@
         <v>10</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
@@ -5768,7 +5769,7 @@
         <v>9</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D90" s="15"/>
       <c r="E90" s="15"/>
@@ -5787,7 +5788,7 @@
         <v>10</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D91" s="15"/>
       <c r="E91" s="15"/>
@@ -6188,7 +6189,7 @@
         <v>109</v>
       </c>
       <c r="D112" s="21" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E112" s="15" t="s">
         <v>110</v>
@@ -6698,7 +6699,7 @@
         <v>26</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="15"/>
@@ -6735,7 +6736,7 @@
         <v>136</v>
       </c>
       <c r="D141" s="24" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E141" s="15" t="s">
         <v>137</v>
@@ -6789,7 +6790,7 @@
         <v>2</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="15"/>
@@ -7585,8 +7586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N218"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7759,26 +7760,26 @@
       <c r="B14" s="4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="48" t="s">
         <v>185</v>
       </c>
       <c r="E14" s="4">
         <v>4.9000000000000004</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>598</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8127,7 +8128,7 @@
         <v>28</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E43" s="4">
         <v>4.1100000000000003</v>
@@ -8175,7 +8176,7 @@
         <v>32</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E47" s="4">
         <v>4.1100000000000003</v>
@@ -8238,10 +8239,10 @@
         <v>4.12</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8315,7 +8316,7 @@
         <v>4.12</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>234</v>
@@ -8326,7 +8327,7 @@
         <v>4.12</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>234</v>
@@ -8359,7 +8360,7 @@
         <v>4.12</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>234</v>
@@ -8418,7 +8419,7 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>240</v>
@@ -8510,7 +8511,7 @@
         <v>4.17</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>243</v>
@@ -8532,8 +8533,8 @@
       <c r="B82" s="4">
         <v>4.1900000000000004</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>1141</v>
+      <c r="C82" s="32" t="s">
+        <v>1139</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8696,7 +8697,7 @@
         <v>260</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="98" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8707,7 +8708,7 @@
         <v>4.25</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>266</v>
@@ -9122,7 +9123,7 @@
         <v>294</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I126" s="4" t="s">
         <v>299</v>
@@ -9140,7 +9141,7 @@
         <v>294</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I127" s="4" t="s">
         <v>300</v>
@@ -9158,10 +9159,10 @@
         <v>294</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I128" s="4" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="129" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9176,7 +9177,7 @@
         <v>294</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I129" s="4" t="s">
         <v>301</v>
@@ -9194,7 +9195,7 @@
         <v>294</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I130" s="4" t="s">
         <v>302</v>
@@ -9212,7 +9213,7 @@
         <v>294</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I131" s="4" t="s">
         <v>303</v>
@@ -9230,7 +9231,7 @@
         <v>294</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I132" s="4" t="s">
         <v>304</v>
@@ -9248,7 +9249,7 @@
         <v>294</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="I133" s="4" t="s">
         <v>305</v>
@@ -9256,7 +9257,7 @@
     </row>
     <row r="134" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E134" s="4" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="135" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9478,7 +9479,7 @@
     <row r="153" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="154" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B154" s="34" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C154" s="34"/>
       <c r="D154" s="34"/>
@@ -9701,8 +9702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
@@ -10022,7 +10023,7 @@
         <v>377</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>374</v>
@@ -10036,7 +10037,7 @@
         <v>378</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>374</v>
@@ -10050,7 +10051,7 @@
         <v>379</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>374</v>
@@ -10172,13 +10173,13 @@
         <v>277</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>1016</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>1017</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>1018</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10192,7 +10193,7 @@
         <v>277</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10206,10 +10207,10 @@
         <v>277</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10223,7 +10224,7 @@
         <v>277</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10237,12 +10238,12 @@
         <v>277</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C38" s="4" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>397</v>
@@ -10251,7 +10252,7 @@
         <v>277</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10295,7 +10296,7 @@
   <dimension ref="A2:Q104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
@@ -10359,7 +10360,7 @@
         <v>367</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10373,7 +10374,7 @@
         <v>367</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10387,7 +10388,7 @@
         <v>367</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10401,7 +10402,7 @@
         <v>367</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10450,7 +10451,7 @@
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>353</v>
@@ -10459,7 +10460,7 @@
         <v>367</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10473,7 +10474,7 @@
         <v>367</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10487,7 +10488,7 @@
         <v>367</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10504,7 +10505,7 @@
         <v>414</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10512,7 +10513,7 @@
         <v>415</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -10521,7 +10522,7 @@
         <v>6.4</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -10869,7 +10870,7 @@
         <v>6.9</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E66" s="41"/>
     </row>
@@ -10907,7 +10908,7 @@
         <v>445</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10915,7 +10916,7 @@
         <v>446</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="74" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10923,7 +10924,7 @@
         <v>447</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10931,7 +10932,7 @@
         <v>442</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10939,7 +10940,7 @@
         <v>448</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="77" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10947,7 +10948,7 @@
         <v>449</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="78" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10955,7 +10956,7 @@
         <v>450</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="79" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10963,7 +10964,7 @@
         <v>451</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="80" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10971,7 +10972,7 @@
         <v>452</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="81" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10979,7 +10980,7 @@
         <v>453</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="82" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10987,7 +10988,7 @@
         <v>454</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="83" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10995,7 +10996,7 @@
         <v>455</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="84" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11003,7 +11004,7 @@
         <v>456</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="85" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -11018,16 +11019,16 @@
         <v>411</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>481</v>
       </c>
       <c r="K86" s="4" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="87" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11038,13 +11039,13 @@
         <v>411</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="88" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11055,10 +11056,10 @@
         <v>411</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="89" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11069,31 +11070,31 @@
         <v>411</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="L89" s="4" t="s">
+        <v>993</v>
+      </c>
+      <c r="M89" s="4" t="s">
+        <v>992</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>994</v>
+      </c>
+      <c r="O89" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="M89" s="4" t="s">
-        <v>994</v>
-      </c>
-      <c r="N89" s="4" t="s">
+      <c r="P89" s="4" t="s">
         <v>996</v>
       </c>
-      <c r="O89" s="4" t="s">
+      <c r="Q89" s="4" t="s">
         <v>997</v>
-      </c>
-      <c r="P89" s="4" t="s">
-        <v>998</v>
-      </c>
-      <c r="Q89" s="4" t="s">
-        <v>999</v>
       </c>
     </row>
     <row r="90" spans="1:17" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11104,25 +11105,25 @@
         <v>411</v>
       </c>
       <c r="F90" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>966</v>
+      </c>
+      <c r="M90" s="4" t="s">
         <v>961</v>
-      </c>
-      <c r="H90" s="4" t="s">
-        <v>964</v>
-      </c>
-      <c r="I90" s="4" t="s">
-        <v>965</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>966</v>
-      </c>
-      <c r="K90" s="4" t="s">
-        <v>967</v>
-      </c>
-      <c r="L90" s="4" t="s">
-        <v>968</v>
-      </c>
-      <c r="M90" s="4" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11134,10 +11135,10 @@
         <v>411</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11149,28 +11150,28 @@
         <v>411</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C93" s="5" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
         <v>411</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11182,64 +11183,64 @@
         <v>411</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C95" s="4" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
         <v>411</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="K95" s="4" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C96" s="5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
         <v>411</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="I96" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="K96" s="4" t="s">
+        <v>987</v>
+      </c>
+      <c r="L96" s="4" t="s">
         <v>988</v>
       </c>
-      <c r="J96" s="4" t="s">
-        <v>843</v>
-      </c>
-      <c r="K96" s="4" t="s">
+      <c r="M96" s="4" t="s">
         <v>989</v>
       </c>
-      <c r="L96" s="4" t="s">
+      <c r="N96" s="4" t="s">
         <v>990</v>
       </c>
-      <c r="M96" s="4" t="s">
-        <v>991</v>
-      </c>
-      <c r="N96" s="4" t="s">
-        <v>992</v>
-      </c>
       <c r="O96" s="4" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="97" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11251,10 +11252,10 @@
         <v>411</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="98" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11266,10 +11267,10 @@
         <v>411</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="99" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11281,10 +11282,10 @@
         <v>411</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="100" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11296,10 +11297,10 @@
         <v>411</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="101" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11311,10 +11312,10 @@
         <v>411</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="102" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11324,7 +11325,7 @@
     </row>
     <row r="103" spans="3:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C103" s="25" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -11345,11 +11346,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D120" sqref="D120"/>
+      <selection pane="bottomRight" activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11390,7 +11391,7 @@
         <v>7.2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>277</v>
@@ -11401,7 +11402,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>277</v>
@@ -11421,7 +11422,7 @@
         <v>399</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11435,7 +11436,7 @@
         <v>399</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11449,7 +11450,7 @@
         <v>399</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11463,13 +11464,13 @@
         <v>399</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11483,7 +11484,7 @@
         <v>399</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11508,7 +11509,7 @@
         <v>399</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11547,7 +11548,7 @@
         <v>492</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -11603,10 +11604,10 @@
         <v>495</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11614,13 +11615,13 @@
         <v>496</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="H29" s="4" t="s">
+        <v>1009</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>1011</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>1013</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>440</v>
@@ -11631,7 +11632,7 @@
         <v>497</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11669,10 +11670,10 @@
         <v>502</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11683,10 +11684,10 @@
         <v>503</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -11701,10 +11702,10 @@
         <v>504</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -11715,10 +11716,10 @@
         <v>506</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12028,7 +12029,7 @@
         <v>617</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>621</v>
@@ -12042,7 +12043,7 @@
         <v>618</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>621</v>
@@ -12056,7 +12057,7 @@
         <v>619</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>621</v>
@@ -12070,7 +12071,7 @@
         <v>620</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>621</v>
@@ -12091,7 +12092,7 @@
         <v>629</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12102,7 +12103,7 @@
         <v>629</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12113,7 +12114,7 @@
         <v>629</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12124,7 +12125,7 @@
         <v>629</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12135,7 +12136,7 @@
         <v>629</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12146,7 +12147,7 @@
         <v>629</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="93" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12155,7 +12156,7 @@
         <v>630</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12163,7 +12164,7 @@
         <v>631</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12171,7 +12172,7 @@
         <v>632</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12179,7 +12180,7 @@
         <v>633</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="98" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12187,7 +12188,7 @@
         <v>634</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12195,7 +12196,7 @@
         <v>635</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12203,7 +12204,7 @@
         <v>636</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="101" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12211,7 +12212,7 @@
         <v>637</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="102" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -12219,23 +12220,23 @@
         <v>638</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="103" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C103" s="4" t="s">
-        <v>639</v>
+        <v>1142</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C104" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12244,24 +12245,24 @@
         <v>9.2200000000000006</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>539</v>
@@ -12270,119 +12271,119 @@
         <v>277</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="108" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B108" s="4" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B109" s="4" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B111" s="4" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C112" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="113" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="114" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="115" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>436</v>
@@ -12391,132 +12392,132 @@
         <v>277</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="G115" s="4" t="s">
+        <v>935</v>
+      </c>
+      <c r="H115" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="I115" s="4" t="s">
         <v>937</v>
       </c>
-      <c r="H115" s="4" t="s">
+      <c r="J115" s="4" t="s">
         <v>938</v>
       </c>
-      <c r="I115" s="4" t="s">
+      <c r="K115" s="4" t="s">
         <v>939</v>
-      </c>
-      <c r="J115" s="4" t="s">
-        <v>940</v>
-      </c>
-      <c r="K115" s="4" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="116" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="117" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="118" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="119" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="120" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C120" s="5" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="121" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="I121" s="4" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="J121" s="4" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="K121" s="4" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="L121" s="4" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="122" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="123" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12525,79 +12526,79 @@
         <v>9.23</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="125" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C125" s="4" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D125" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="126" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C126" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="127" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C127" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="128" spans="1:12" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C128" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="129" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C129" s="4" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="130" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C130" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="131" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12612,18 +12613,18 @@
         <v>277</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="133" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C133" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>277</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="134" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12643,7 +12644,7 @@
     </row>
     <row r="136" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E136" s="4" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="F136" s="4" t="s">
         <v>399</v>
@@ -12670,40 +12671,40 @@
         <v>13.5</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="G139" s="4" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="140" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G140" s="4" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="141" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G141" s="4" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="142" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G142" s="4" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="143" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G143" s="4" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="144" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G144" s="4" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="145" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G145" s="4" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="146" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12866,10 +12867,10 @@
   <dimension ref="A2:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13639,7 +13640,7 @@
     <row r="86" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C87" s="38" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13650,7 +13651,7 @@
         <v>602</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13658,7 +13659,7 @@
         <v>560</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13666,7 +13667,7 @@
         <v>603</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13674,7 +13675,7 @@
         <v>604</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13682,7 +13683,7 @@
         <v>541</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13722,7 +13723,7 @@
     </row>
     <row r="99" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="100" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A100" s="4">
+      <c r="A100" s="32">
         <v>9.16</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -13753,6 +13754,9 @@
       </c>
     </row>
     <row r="102" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A102" s="4">
+        <v>9.17</v>
+      </c>
       <c r="C102" s="4" t="s">
         <v>606</v>
       </c>
@@ -13781,10 +13785,10 @@
   <dimension ref="A2:P203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C158" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C126" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D163" sqref="D163"/>
+      <selection pane="bottomRight" activeCell="C131" sqref="C131:D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13804,7 +13808,7 @@
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13813,10 +13817,10 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>343</v>
@@ -13825,7 +13829,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13833,10 +13837,10 @@
         <v>12.2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13844,10 +13848,10 @@
         <v>12.3</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>667</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>668</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>399</v>
@@ -13855,10 +13859,10 @@
     </row>
     <row r="8" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>399</v>
@@ -13866,10 +13870,10 @@
     </row>
     <row r="9" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G9" s="29" t="s">
         <v>399</v>
@@ -13877,10 +13881,10 @@
     </row>
     <row r="10" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>399</v>
@@ -13892,46 +13896,46 @@
         <v>12.4</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C13" s="29" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C14" s="29" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C15" s="29" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -13940,10 +13944,10 @@
         <v>12.5</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>615</v>
@@ -13951,10 +13955,10 @@
     </row>
     <row r="18" spans="1:14" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C18" s="29" t="s">
+        <v>682</v>
+      </c>
+      <c r="F18" s="29" t="s">
         <v>683</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>684</v>
       </c>
       <c r="G18" s="29" t="s">
         <v>615</v>
@@ -13966,58 +13970,58 @@
         <v>12.6</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H20" s="44" t="s">
+        <v>1046</v>
+      </c>
+      <c r="I20" s="45" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J20" s="44" t="s">
         <v>1048</v>
       </c>
-      <c r="I20" s="45" t="s">
+      <c r="K20" s="44" t="s">
         <v>1049</v>
       </c>
-      <c r="J20" s="44" t="s">
+      <c r="L20" s="44" t="s">
         <v>1050</v>
       </c>
-      <c r="K20" s="44" t="s">
+      <c r="M20" s="44" t="s">
         <v>1051</v>
       </c>
-      <c r="L20" s="44" t="s">
+      <c r="N20" s="44" t="s">
         <v>1052</v>
-      </c>
-      <c r="M20" s="44" t="s">
-        <v>1053</v>
-      </c>
-      <c r="N20" s="44" t="s">
-        <v>1054</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H21" s="44" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H22" s="44" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D23" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H23" s="44" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="I23" s="44" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14025,10 +14029,10 @@
         <v>12.7</v>
       </c>
       <c r="C24" s="29" t="s">
+        <v>728</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>729</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>730</v>
       </c>
       <c r="G24" s="29" t="s">
         <v>615</v>
@@ -14036,7 +14040,7 @@
     </row>
     <row r="25" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E25" s="4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G25" s="29" t="s">
         <v>615</v>
@@ -14044,7 +14048,7 @@
     </row>
     <row r="26" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E26" s="4" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G26" s="29" t="s">
         <v>615</v>
@@ -14052,7 +14056,7 @@
     </row>
     <row r="27" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E27" s="4" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="G27" s="29" t="s">
         <v>615</v>
@@ -14060,7 +14064,7 @@
     </row>
     <row r="28" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E28" s="4" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G28" s="29" t="s">
         <v>615</v>
@@ -14068,7 +14072,7 @@
     </row>
     <row r="29" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E29" s="4" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G29" s="29" t="s">
         <v>615</v>
@@ -14076,7 +14080,7 @@
     </row>
     <row r="30" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E30" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G30" s="29" t="s">
         <v>615</v>
@@ -14084,7 +14088,7 @@
     </row>
     <row r="31" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E31" s="4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G31" s="29" t="s">
         <v>615</v>
@@ -14092,7 +14096,7 @@
     </row>
     <row r="32" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E32" s="4" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G32" s="29" t="s">
         <v>615</v>
@@ -14100,7 +14104,7 @@
     </row>
     <row r="33" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E33" s="4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G33" s="29" t="s">
         <v>615</v>
@@ -14108,7 +14112,7 @@
     </row>
     <row r="34" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E34" s="4" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="G34" s="29" t="s">
         <v>615</v>
@@ -14116,7 +14120,7 @@
     </row>
     <row r="35" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E35" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G35" s="29" t="s">
         <v>615</v>
@@ -14124,7 +14128,7 @@
     </row>
     <row r="36" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E36" s="4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G36" s="29" t="s">
         <v>615</v>
@@ -14132,7 +14136,7 @@
     </row>
     <row r="37" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E37" s="4" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G37" s="29" t="s">
         <v>615</v>
@@ -14140,7 +14144,7 @@
     </row>
     <row r="38" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E38" s="4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="G38" s="29" t="s">
         <v>615</v>
@@ -14148,7 +14152,7 @@
     </row>
     <row r="39" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E39" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="G39" s="29" t="s">
         <v>615</v>
@@ -14156,7 +14160,7 @@
     </row>
     <row r="40" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E40" s="4" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="G40" s="29" t="s">
         <v>615</v>
@@ -14164,7 +14168,7 @@
     </row>
     <row r="41" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E41" s="4" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="G41" s="29" t="s">
         <v>615</v>
@@ -14172,7 +14176,7 @@
     </row>
     <row r="42" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E42" s="4" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="G42" s="29" t="s">
         <v>615</v>
@@ -14180,7 +14184,7 @@
     </row>
     <row r="43" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E43" s="4" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G43" s="29" t="s">
         <v>615</v>
@@ -14188,7 +14192,7 @@
     </row>
     <row r="44" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E44" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="G44" s="29" t="s">
         <v>615</v>
@@ -14196,7 +14200,7 @@
     </row>
     <row r="45" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E45" s="4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G45" s="29" t="s">
         <v>615</v>
@@ -14204,7 +14208,7 @@
     </row>
     <row r="46" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E46" s="4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G46" s="29" t="s">
         <v>615</v>
@@ -14212,7 +14216,7 @@
     </row>
     <row r="47" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E47" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G47" s="29" t="s">
         <v>615</v>
@@ -14220,7 +14224,7 @@
     </row>
     <row r="48" spans="5:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E48" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G48" s="29" t="s">
         <v>615</v>
@@ -14228,7 +14232,7 @@
     </row>
     <row r="49" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E49" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G49" s="29" t="s">
         <v>615</v>
@@ -14236,7 +14240,7 @@
     </row>
     <row r="50" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E50" s="4" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G50" s="29" t="s">
         <v>615</v>
@@ -14244,7 +14248,7 @@
     </row>
     <row r="51" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E51" s="4" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G51" s="29" t="s">
         <v>615</v>
@@ -14252,7 +14256,7 @@
     </row>
     <row r="52" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E52" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G52" s="29" t="s">
         <v>615</v>
@@ -14260,7 +14264,7 @@
     </row>
     <row r="53" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E53" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G53" s="29" t="s">
         <v>615</v>
@@ -14271,7 +14275,7 @@
         <v>12.8</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="G54" s="29" t="s">
         <v>615</v>
@@ -14279,7 +14283,7 @@
     </row>
     <row r="55" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D55" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G55" s="29" t="s">
         <v>615</v>
@@ -14287,7 +14291,7 @@
     </row>
     <row r="56" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D56" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G56" s="29" t="s">
         <v>615</v>
@@ -14295,7 +14299,7 @@
     </row>
     <row r="57" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D57" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="G57" s="29" t="s">
         <v>615</v>
@@ -14303,7 +14307,7 @@
     </row>
     <row r="58" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D58" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="G58" s="29" t="s">
         <v>615</v>
@@ -14311,7 +14315,7 @@
     </row>
     <row r="59" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D59" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="G59" s="29" t="s">
         <v>615</v>
@@ -14319,7 +14323,7 @@
     </row>
     <row r="60" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D60" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="G60" s="29" t="s">
         <v>615</v>
@@ -14327,7 +14331,7 @@
     </row>
     <row r="61" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D61" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G61" s="29" t="s">
         <v>615</v>
@@ -14335,7 +14339,7 @@
     </row>
     <row r="62" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D62" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="G62" s="29" t="s">
         <v>615</v>
@@ -14343,7 +14347,7 @@
     </row>
     <row r="63" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D63" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="G63" s="29" t="s">
         <v>615</v>
@@ -14351,7 +14355,7 @@
     </row>
     <row r="64" spans="1:7" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D64" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G64" s="29" t="s">
         <v>615</v>
@@ -14359,7 +14363,7 @@
     </row>
     <row r="65" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G65" s="29" t="s">
         <v>615</v>
@@ -14367,7 +14371,7 @@
     </row>
     <row r="66" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="G66" s="29" t="s">
         <v>615</v>
@@ -14375,7 +14379,7 @@
     </row>
     <row r="67" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D67" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G67" s="29" t="s">
         <v>615</v>
@@ -14384,7 +14388,7 @@
     <row r="68" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="69" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B69" s="30"/>
       <c r="C69" s="30">
@@ -14397,18 +14401,18 @@
         <v>11.3</v>
       </c>
       <c r="C71" s="29" t="s">
+        <v>731</v>
+      </c>
+      <c r="F71" s="29" t="s">
         <v>732</v>
       </c>
-      <c r="F71" s="29" t="s">
-        <v>733</v>
-      </c>
       <c r="H71" s="29" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C72" s="29" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F72" s="29" t="s">
         <v>303</v>
@@ -14422,55 +14426,55 @@
     </row>
     <row r="73" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C73" s="29" t="s">
+        <v>733</v>
+      </c>
+      <c r="F73" s="29" t="s">
         <v>734</v>
-      </c>
-      <c r="F73" s="29" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="74" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C74" s="29" t="s">
+        <v>735</v>
+      </c>
+      <c r="F74" s="29" t="s">
         <v>736</v>
       </c>
-      <c r="F74" s="29" t="s">
-        <v>737</v>
-      </c>
       <c r="H74" s="42" t="s">
+        <v>1042</v>
+      </c>
+      <c r="I74" s="42" t="s">
+        <v>930</v>
+      </c>
+      <c r="J74" s="42" t="s">
+        <v>1043</v>
+      </c>
+      <c r="K74" s="42" t="s">
         <v>1044</v>
-      </c>
-      <c r="I74" s="42" t="s">
-        <v>932</v>
-      </c>
-      <c r="J74" s="42" t="s">
-        <v>1045</v>
-      </c>
-      <c r="K74" s="42" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C75" s="29" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F75" s="29" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H75" s="42" t="s">
+        <v>1032</v>
+      </c>
+      <c r="I75" s="44" t="s">
+        <v>1033</v>
+      </c>
+      <c r="J75" s="42" t="s">
         <v>1034</v>
-      </c>
-      <c r="I75" s="44" t="s">
-        <v>1035</v>
-      </c>
-      <c r="J75" s="42" t="s">
-        <v>1036</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C76" s="29" t="s">
+        <v>738</v>
+      </c>
+      <c r="F76" s="29" t="s">
         <v>739</v>
-      </c>
-      <c r="F76" s="29" t="s">
-        <v>740</v>
       </c>
       <c r="H76" s="29">
         <v>5.0999999999999996</v>
@@ -14478,98 +14482,98 @@
     </row>
     <row r="77" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C77" s="29" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F77" s="29" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="H77" s="42" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C78" s="29" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F78" s="29" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="H78" s="44" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C79" s="29" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F79" s="29" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H79" s="44" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I79" s="42" t="s">
+        <v>1039</v>
+      </c>
+      <c r="J79" s="43" t="s">
         <v>1040</v>
       </c>
-      <c r="I79" s="42" t="s">
+      <c r="K79" s="43" t="s">
         <v>1041</v>
-      </c>
-      <c r="J79" s="43" t="s">
-        <v>1042</v>
-      </c>
-      <c r="K79" s="43" t="s">
-        <v>1043</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C80" s="29" t="s">
+        <v>743</v>
+      </c>
+      <c r="F80" s="29" t="s">
         <v>744</v>
-      </c>
-      <c r="F80" s="29" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C81" s="29" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C82" s="29" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="I82" s="29" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C83" s="29" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C84" s="29" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C85" s="29" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -14578,32 +14582,32 @@
         <v>11.4</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E88" s="4" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="89" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E89" s="4" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E90" s="4" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E91" s="4" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E92" s="4" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14611,97 +14615,97 @@
         <v>11.5</v>
       </c>
       <c r="C93" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="D93" s="4" t="s">
         <v>757</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>758</v>
       </c>
       <c r="G93" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H93" s="45" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="C94" s="4" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H94" s="45" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C95" s="4" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G95" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H95" s="45" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C96" s="4" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G96" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H96" s="45" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="97" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C97" s="6" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C98" s="4" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G98" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H98" s="45" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="99" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C99" s="4" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G99" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H99" s="45" t="s">
+        <v>1058</v>
+      </c>
+      <c r="I99" s="45" t="s">
+        <v>1059</v>
+      </c>
+      <c r="J99" s="45" t="s">
         <v>1060</v>
-      </c>
-      <c r="I99" s="45" t="s">
-        <v>1061</v>
-      </c>
-      <c r="J99" s="45" t="s">
-        <v>1062</v>
       </c>
     </row>
     <row r="100" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -14710,30 +14714,30 @@
         <v>11.6</v>
       </c>
       <c r="C101" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="D101" s="4" t="s">
         <v>763</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>764</v>
       </c>
       <c r="G101" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H101" s="45" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="102" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C102" s="4" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G102" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H102" s="45" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="103" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -14742,30 +14746,30 @@
         <v>11.7</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G104" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H104" s="45" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="105" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C105" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>765</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>766</v>
       </c>
       <c r="G105" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H105" s="45" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="106" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14780,7 +14784,7 @@
         <v>263</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="108" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14788,22 +14792,22 @@
         <v>263</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G108" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H108" s="45" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I108" s="45" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J108" s="45" t="s">
         <v>1065</v>
       </c>
-      <c r="I108" s="45" t="s">
+      <c r="K108" s="45" t="s">
         <v>1066</v>
-      </c>
-      <c r="J108" s="45" t="s">
-        <v>1067</v>
-      </c>
-      <c r="K108" s="45" t="s">
-        <v>1068</v>
       </c>
     </row>
     <row r="109" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14811,13 +14815,13 @@
         <v>263</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G109" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H109" s="45" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="110" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -14826,16 +14830,16 @@
         <v>11.9</v>
       </c>
       <c r="C111" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="D111" s="4" t="s">
         <v>770</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>771</v>
       </c>
       <c r="G111" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H111" s="45" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="112" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14843,7 +14847,7 @@
         <v>378</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="113" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14851,13 +14855,13 @@
         <v>502</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G113" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H113" s="45" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="114" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14873,140 +14877,152 @@
         <v>11.1</v>
       </c>
       <c r="C116" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="D116" s="4" t="s">
         <v>772</v>
       </c>
-      <c r="D116" s="4" t="s">
-        <v>773</v>
+      <c r="G116" s="29" t="s">
+        <v>399</v>
       </c>
       <c r="H116" s="44" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="I116" s="44" t="s">
+        <v>1070</v>
+      </c>
+      <c r="J116" s="44" t="s">
+        <v>1071</v>
+      </c>
+      <c r="K116" s="44" t="s">
         <v>1072</v>
       </c>
-      <c r="J116" s="44" t="s">
+      <c r="L116" s="44" t="s">
         <v>1073</v>
-      </c>
-      <c r="K116" s="44" t="s">
-        <v>1074</v>
-      </c>
-      <c r="L116" s="44" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="117" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C117" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>774</v>
+        <v>773</v>
+      </c>
+      <c r="G117" s="29" t="s">
+        <v>399</v>
       </c>
       <c r="H117" s="44" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="I117" s="44" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="118" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C118" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>775</v>
+        <v>774</v>
+      </c>
+      <c r="G118" s="29" t="s">
+        <v>399</v>
       </c>
       <c r="H118" s="44" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="119" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C119" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>776</v>
+        <v>775</v>
+      </c>
+      <c r="G119" s="29" t="s">
+        <v>399</v>
       </c>
       <c r="H119" s="44" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I119" s="44" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J119" s="44" t="s">
         <v>1080</v>
       </c>
-      <c r="I119" s="44" t="s">
+      <c r="K119" s="44" t="s">
         <v>1081</v>
       </c>
-      <c r="J119" s="44" t="s">
+      <c r="L119" s="44" t="s">
         <v>1082</v>
       </c>
-      <c r="K119" s="44" t="s">
+      <c r="M119" s="44" t="s">
         <v>1083</v>
       </c>
-      <c r="L119" s="44" t="s">
+      <c r="N119" s="44" t="s">
         <v>1084</v>
       </c>
-      <c r="M119" s="44" t="s">
+      <c r="O119" s="44" t="s">
         <v>1085</v>
       </c>
-      <c r="N119" s="44" t="s">
+      <c r="P119" s="44" t="s">
         <v>1086</v>
-      </c>
-      <c r="O119" s="44" t="s">
-        <v>1087</v>
-      </c>
-      <c r="P119" s="44" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="120" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="H120" s="44" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="I120" s="44" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J120" s="44" t="s">
+        <v>1088</v>
+      </c>
+      <c r="K120" s="44" t="s">
         <v>1089</v>
       </c>
-      <c r="J120" s="44" t="s">
+      <c r="L120" s="44" t="s">
         <v>1090</v>
       </c>
-      <c r="K120" s="44" t="s">
+      <c r="M120" s="44" t="s">
+        <v>962</v>
+      </c>
+      <c r="N120" s="44" t="s">
         <v>1091</v>
       </c>
-      <c r="L120" s="44" t="s">
+      <c r="O120" s="44" t="s">
         <v>1092</v>
       </c>
-      <c r="M120" s="44" t="s">
-        <v>964</v>
-      </c>
-      <c r="N120" s="44" t="s">
+      <c r="P120" s="44" t="s">
         <v>1093</v>
-      </c>
-      <c r="O120" s="44" t="s">
-        <v>1094</v>
-      </c>
-      <c r="P120" s="44" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="121" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="H121" s="44" t="s">
+        <v>1094</v>
+      </c>
+      <c r="I121" s="44" t="s">
+        <v>1095</v>
+      </c>
+      <c r="J121" s="44" t="s">
         <v>1096</v>
       </c>
-      <c r="I121" s="44" t="s">
+      <c r="K121" s="44" t="s">
         <v>1097</v>
       </c>
-      <c r="J121" s="44" t="s">
+      <c r="L121" s="44" t="s">
         <v>1098</v>
       </c>
-      <c r="K121" s="44" t="s">
+      <c r="M121" s="44" t="s">
         <v>1099</v>
       </c>
-      <c r="L121" s="44" t="s">
+      <c r="N121" s="44" t="s">
         <v>1100</v>
       </c>
-      <c r="M121" s="44" t="s">
+      <c r="O121" s="44" t="s">
         <v>1101</v>
-      </c>
-      <c r="N121" s="44" t="s">
-        <v>1102</v>
-      </c>
-      <c r="O121" s="44" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="122" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -15015,25 +15031,25 @@
         <v>11.11</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H123" s="44" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I123" s="44" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J123" s="44" t="s">
         <v>1104</v>
       </c>
-      <c r="I123" s="44" t="s">
+      <c r="K123" s="44" t="s">
         <v>1105</v>
       </c>
-      <c r="J123" s="44" t="s">
+      <c r="L123" s="44" t="s">
         <v>1106</v>
-      </c>
-      <c r="K123" s="44" t="s">
-        <v>1107</v>
-      </c>
-      <c r="L123" s="44" t="s">
-        <v>1108</v>
       </c>
     </row>
     <row r="124" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15041,41 +15057,41 @@
         <v>11.12</v>
       </c>
       <c r="C124" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="D124" s="4" t="s">
         <v>777</v>
       </c>
-      <c r="D124" s="4" t="s">
-        <v>778</v>
-      </c>
       <c r="H124" s="44" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="125" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C125" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H125" s="44" t="s">
+        <v>1107</v>
+      </c>
+      <c r="I125" s="43" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J125" s="43" t="s">
         <v>1109</v>
-      </c>
-      <c r="I125" s="43" t="s">
-        <v>1110</v>
-      </c>
-      <c r="J125" s="43" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="126" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C126" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H126" s="44" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="127" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -15084,127 +15100,127 @@
         <v>11.13</v>
       </c>
       <c r="C128" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>781</v>
       </c>
-      <c r="D128" s="4" t="s">
-        <v>782</v>
-      </c>
       <c r="H128" s="44" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="I128" s="44" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="129" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C129" s="4" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>416</v>
       </c>
       <c r="H129" s="44" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I129" s="43" t="s">
+        <v>925</v>
+      </c>
+      <c r="J129" s="44" t="s">
+        <v>951</v>
+      </c>
+      <c r="K129" s="44" t="s">
+        <v>1115</v>
+      </c>
+      <c r="L129" s="43" t="s">
         <v>1116</v>
       </c>
-      <c r="I129" s="43" t="s">
-        <v>927</v>
-      </c>
-      <c r="J129" s="44" t="s">
-        <v>953</v>
-      </c>
-      <c r="K129" s="44" t="s">
-        <v>1117</v>
-      </c>
-      <c r="L129" s="43" t="s">
-        <v>1118</v>
-      </c>
       <c r="M129" s="29" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="130" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C130" s="4" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D130" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="H130" s="44" t="s">
+        <v>1117</v>
+      </c>
+      <c r="I130" s="44" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C131" s="32" t="s">
+        <v>780</v>
+      </c>
+      <c r="D131" s="32" t="s">
         <v>783</v>
       </c>
-      <c r="H130" s="44" t="s">
+      <c r="H131" s="44" t="s">
         <v>1119</v>
       </c>
-      <c r="I130" s="44" t="s">
+      <c r="I131" s="44" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C131" s="4" t="s">
-        <v>781</v>
-      </c>
-      <c r="D131" s="4" t="s">
-        <v>784</v>
-      </c>
-      <c r="H131" s="44" t="s">
+      <c r="J131" s="44" t="s">
         <v>1121</v>
-      </c>
-      <c r="I131" s="44" t="s">
-        <v>1122</v>
-      </c>
-      <c r="J131" s="44" t="s">
-        <v>1123</v>
       </c>
     </row>
     <row r="132" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C132" s="4" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H132" s="44" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="I132" s="44" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="133" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C133" s="4" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H133" s="44" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="I133" s="44" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="134" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C134" s="4" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H134" s="46" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I134" s="46" t="s">
+        <v>1125</v>
+      </c>
+      <c r="J134" s="46" t="s">
         <v>1126</v>
       </c>
-      <c r="I134" s="46" t="s">
+      <c r="K134" s="46" t="s">
         <v>1127</v>
       </c>
-      <c r="J134" s="46" t="s">
+      <c r="L134" s="43" t="s">
         <v>1128</v>
       </c>
-      <c r="K134" s="46" t="s">
+      <c r="M134" s="46" t="s">
         <v>1129</v>
-      </c>
-      <c r="L134" s="43" t="s">
-        <v>1130</v>
-      </c>
-      <c r="M134" s="46" t="s">
-        <v>1131</v>
       </c>
     </row>
     <row r="135" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -15216,19 +15232,19 @@
         <v>300</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="137" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C137" s="4"/>
       <c r="D137" s="4" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="138" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C138" s="4"/>
       <c r="D138" s="4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="139" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -15237,24 +15253,24 @@
         <v>11.15</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>416</v>
       </c>
       <c r="H140" s="44" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="141" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C141" s="4" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>416</v>
       </c>
       <c r="H141" s="44" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="142" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -15263,137 +15279,137 @@
         <v>11.16</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="144" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D144" s="4" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="145" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D145" s="4" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="146" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D146" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="147" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D147" s="4" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="148" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D148" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="149" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D149" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="150" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D150" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="151" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D151" s="4" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="152" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D152" s="4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="153" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D153" s="4" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="154" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D154" s="4" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="155" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D155" s="4" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="156" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D156" s="4" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="157" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D157" s="4" t="s">
-        <v>1134</v>
+      <c r="D157" s="32" t="s">
+        <v>1132</v>
       </c>
     </row>
     <row r="158" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D158" s="4" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="159" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D159" s="4" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="160" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D160" s="4" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="161" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D161" s="4" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="162" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D162" s="4" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D163" s="32" t="s">
         <v>808</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D163" s="4" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="164" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D164" s="4" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="165" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D165" s="4" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="166" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D166" s="4" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="167" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D167" s="4" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="168" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D168" s="4" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D169" s="4" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15401,127 +15417,127 @@
         <v>11.17</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E172" s="4" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E173" s="4" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E174" s="4" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E175" s="4" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E176" s="4" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="177" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E177" s="4" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="178" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E178" s="4" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="179" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E179" s="4" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="180" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E180" s="4" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="181" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E181" s="4" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="182" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E182" s="4" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="183" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E183" s="4" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="184" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E184" s="4" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="185" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E185" s="4" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="186" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E186" s="4" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="187" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E187" s="4" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="188" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E188" s="4" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="189" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E189" s="4" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="190" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E190" s="4" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="191" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E191" s="4" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="192" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E192" s="4" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="193" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E193" s="4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="194" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E194" s="4" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="195" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E195" s="4" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="196" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15529,10 +15545,10 @@
         <v>11.18</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>841</v>
+        <v>1141</v>
       </c>
       <c r="F196" s="4" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="197" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -15571,10 +15587,10 @@
     </row>
     <row r="3" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -15585,19 +15601,19 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>343</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15605,58 +15621,58 @@
         <v>16.2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>851</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>853</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>852</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>853</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>736</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -15665,7 +15681,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -15674,10 +15690,10 @@
         <v>16.5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15685,7 +15701,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -15694,18 +15710,18 @@
         <v>16.7</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>859</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C18" s="4" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -15714,10 +15730,10 @@
         <v>16.8</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15725,10 +15741,10 @@
         <v>16.899999999999999</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>862</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15736,10 +15752,10 @@
         <v>16.899999999999999</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15747,7 +15763,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15755,7 +15771,7 @@
         <v>16.11</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15763,34 +15779,34 @@
         <v>16.12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C26" s="4" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C27" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>870</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C28" s="4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -15799,18 +15815,18 @@
         <v>16.25</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>873</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C31" s="4" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15818,7 +15834,7 @@
         <v>489</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -15827,35 +15843,35 @@
         <v>16.27</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C35" s="4" t="s">
+        <v>875</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>877</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>879</v>
-      </c>
       <c r="G35" s="4" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C36" s="4" t="s">
+        <v>876</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>877</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>878</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>879</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -15867,21 +15883,21 @@
         <v>351</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C39" s="4" t="s">
+        <v>879</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>880</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>881</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>882</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Jatai and Ghanam related working files 31/01/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Avagraha" sheetId="7" r:id="rId7"/>
     <sheet name="Special Anuswaram" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4180,8 +4180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L192"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7586,8 +7586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N218"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B122" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9703,7 +9703,7 @@
   <dimension ref="A2:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
@@ -10296,7 +10296,7 @@
   <dimension ref="A2:Q104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
@@ -11347,10 +11347,10 @@
   <dimension ref="A3:L294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D131" sqref="D131"/>
+      <selection pane="bottomRight" activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12867,10 +12867,10 @@
   <dimension ref="A2:G109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="L100" sqref="L100"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13785,10 +13785,10 @@
   <dimension ref="A2:P203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C126" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C164" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C131" sqref="C131:D131"/>
+      <selection pane="bottomRight" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
New Sandhi Rule Sandhi chart 27/04/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="1188">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -3330,9 +3330,6 @@
     <t>6.1.7.2</t>
   </si>
   <si>
-    <t>3.2?</t>
-  </si>
-  <si>
     <t>1.5.10.1</t>
   </si>
   <si>
@@ -3622,13 +3619,151 @@
   </si>
   <si>
     <t>poShAn</t>
+  </si>
+  <si>
+    <t>1.1.14</t>
+  </si>
+  <si>
+    <t>1.2.14</t>
+  </si>
+  <si>
+    <t>1.3.14</t>
+  </si>
+  <si>
+    <t>1.4.46</t>
+  </si>
+  <si>
+    <t>1.5.11</t>
+  </si>
+  <si>
+    <t>1.6.12</t>
+  </si>
+  <si>
+    <t>1.7.7</t>
+  </si>
+  <si>
+    <t>1.7.8</t>
+  </si>
+  <si>
+    <t>1.7.9</t>
+  </si>
+  <si>
+    <t>1.7.10</t>
+  </si>
+  <si>
+    <t>1.7.11</t>
+  </si>
+  <si>
+    <t>1.7.12</t>
+  </si>
+  <si>
+    <t>1.7.13</t>
+  </si>
+  <si>
+    <t>1.8.22</t>
+  </si>
+  <si>
+    <t>2.1.11</t>
+  </si>
+  <si>
+    <t>2.2.12</t>
+  </si>
+  <si>
+    <t>2.3.14</t>
+  </si>
+  <si>
+    <t>2.4.14</t>
+  </si>
+  <si>
+    <t>2.5.12</t>
+  </si>
+  <si>
+    <t>2.6.11</t>
+  </si>
+  <si>
+    <t>2.6.12</t>
+  </si>
+  <si>
+    <t>3.1.11</t>
+  </si>
+  <si>
+    <t>3.2.11</t>
+  </si>
+  <si>
+    <t>3.3.11</t>
+  </si>
+  <si>
+    <t>3.4.11</t>
+  </si>
+  <si>
+    <t>3.5.11</t>
+  </si>
+  <si>
+    <t>4.1.11</t>
+  </si>
+  <si>
+    <t>4.2.11</t>
+  </si>
+  <si>
+    <t>4.3.13</t>
+  </si>
+  <si>
+    <t>5.6.1</t>
+  </si>
+  <si>
+    <t>4.6.1</t>
+  </si>
+  <si>
+    <t>4.6.2</t>
+  </si>
+  <si>
+    <t>4.6.3</t>
+  </si>
+  <si>
+    <t>4.6.4</t>
+  </si>
+  <si>
+    <t>4.6.5</t>
+  </si>
+  <si>
+    <t>4.7.12</t>
+  </si>
+  <si>
+    <t>4.7.13</t>
+  </si>
+  <si>
+    <t>4.7.15</t>
+  </si>
+  <si>
+    <t>4.4.12</t>
+  </si>
+  <si>
+    <t>4.4.13</t>
+  </si>
+  <si>
+    <t>4.4.14</t>
+  </si>
+  <si>
+    <t>4.5.1</t>
+  </si>
+  <si>
+    <t>4.5.2</t>
+  </si>
+  <si>
+    <t>4.5.3</t>
+  </si>
+  <si>
+    <t>4.5.4</t>
+  </si>
+  <si>
+    <t>4.5.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3744,6 +3879,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -3822,7 +3962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3898,6 +4038,7 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7767,19 +7908,19 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="K14" s="4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>1133</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>1134</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>598</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8242,7 +8383,7 @@
         <v>916</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -8534,7 +8675,7 @@
         <v>4.1900000000000004</v>
       </c>
       <c r="C82" s="32" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -9123,7 +9264,7 @@
         <v>294</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="I126" s="4" t="s">
         <v>299</v>
@@ -9141,7 +9282,7 @@
         <v>294</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="I127" s="4" t="s">
         <v>300</v>
@@ -9159,7 +9300,7 @@
         <v>294</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="I128" s="4" t="s">
         <v>903</v>
@@ -9177,7 +9318,7 @@
         <v>294</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="I129" s="4" t="s">
         <v>301</v>
@@ -9195,7 +9336,7 @@
         <v>294</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="I130" s="4" t="s">
         <v>302</v>
@@ -9213,7 +9354,7 @@
         <v>294</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="I131" s="4" t="s">
         <v>303</v>
@@ -9231,7 +9372,7 @@
         <v>294</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="I132" s="4" t="s">
         <v>304</v>
@@ -9249,7 +9390,7 @@
         <v>294</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="I133" s="4" t="s">
         <v>305</v>
@@ -9257,7 +9398,7 @@
     </row>
     <row r="134" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E134" s="4" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="135" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -10295,7 +10436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -12225,7 +12366,7 @@
     </row>
     <row r="103" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C103" s="4" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="F103" s="4" t="s">
         <v>841</v>
@@ -13782,13 +13923,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P203"/>
+  <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C164" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="E69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D64" sqref="D64"/>
+      <selection pane="bottomRight" activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13976,25 +14117,25 @@
         <v>684</v>
       </c>
       <c r="H20" s="44" t="s">
+        <v>1045</v>
+      </c>
+      <c r="I20" s="45" t="s">
         <v>1046</v>
       </c>
-      <c r="I20" s="45" t="s">
+      <c r="J20" s="44" t="s">
         <v>1047</v>
       </c>
-      <c r="J20" s="44" t="s">
+      <c r="K20" s="44" t="s">
         <v>1048</v>
       </c>
-      <c r="K20" s="44" t="s">
+      <c r="L20" s="44" t="s">
         <v>1049</v>
       </c>
-      <c r="L20" s="44" t="s">
+      <c r="M20" s="44" t="s">
         <v>1050</v>
       </c>
-      <c r="M20" s="44" t="s">
+      <c r="N20" s="44" t="s">
         <v>1051</v>
-      </c>
-      <c r="N20" s="44" t="s">
-        <v>1052</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14002,7 +14143,7 @@
         <v>685</v>
       </c>
       <c r="H21" s="44" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14010,7 +14151,7 @@
         <v>686</v>
       </c>
       <c r="H22" s="44" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14018,10 +14159,10 @@
         <v>687</v>
       </c>
       <c r="H23" s="44" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="I23" s="44" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14361,7 +14502,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
         <v>726</v>
       </c>
@@ -14369,7 +14510,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
         <v>923</v>
       </c>
@@ -14377,7 +14518,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D67" s="4" t="s">
         <v>727</v>
       </c>
@@ -14385,8 +14526,8 @@
         <v>615</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>730</v>
       </c>
@@ -14395,8 +14536,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="29">
         <v>11.3</v>
       </c>
@@ -14410,7 +14551,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C72" s="29" t="s">
         <v>731</v>
       </c>
@@ -14424,15 +14565,33 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C73" s="29" t="s">
         <v>733</v>
       </c>
       <c r="F73" s="29" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H73" s="29" t="s">
+        <v>1148</v>
+      </c>
+      <c r="I73" s="29" t="s">
+        <v>1149</v>
+      </c>
+      <c r="J73" s="29" t="s">
+        <v>1150</v>
+      </c>
+      <c r="K73" s="29" t="s">
+        <v>1151</v>
+      </c>
+      <c r="L73" s="29" t="s">
+        <v>1152</v>
+      </c>
+      <c r="M73" s="29" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C74" s="29" t="s">
         <v>735</v>
       </c>
@@ -14452,7 +14611,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C75" s="29" t="s">
         <v>735</v>
       </c>
@@ -14469,18 +14628,21 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C76" s="29" t="s">
         <v>738</v>
       </c>
       <c r="F76" s="29" t="s">
         <v>739</v>
       </c>
-      <c r="H76" s="29">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H76" s="49">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I76" s="29">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C77" s="29" t="s">
         <v>735</v>
       </c>
@@ -14491,7 +14653,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C78" s="29" t="s">
         <v>735</v>
       </c>
@@ -14502,7 +14664,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C79" s="29" t="s">
         <v>735</v>
       </c>
@@ -14522,7 +14684,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C80" s="29" t="s">
         <v>743</v>
       </c>
@@ -14530,26 +14692,50 @@
         <v>744</v>
       </c>
     </row>
-    <row r="81" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C81" s="29" t="s">
         <v>733</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H81" s="29" t="s">
+        <v>1172</v>
+      </c>
+      <c r="I81" s="29" t="s">
+        <v>1173</v>
+      </c>
+      <c r="J81" s="29" t="s">
+        <v>1174</v>
+      </c>
+      <c r="K81" s="29" t="s">
+        <v>1175</v>
+      </c>
+      <c r="L81" s="29" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C82" s="29" t="s">
         <v>733</v>
       </c>
       <c r="F82" s="4" t="s">
         <v>748</v>
       </c>
+      <c r="H82" s="29" t="s">
+        <v>1177</v>
+      </c>
       <c r="I82" s="29" t="s">
+        <v>1178</v>
+      </c>
+      <c r="J82" s="29" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K82" s="30" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C83" s="29" t="s">
         <v>733</v>
       </c>
@@ -14557,104 +14743,188 @@
         <v>746</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C84" s="29" t="s">
         <v>733</v>
       </c>
       <c r="F84" s="4" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C85" s="29" t="s">
+      <c r="H84" s="29" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I84" s="29" t="s">
+        <v>1143</v>
+      </c>
+      <c r="J84" s="29" t="s">
+        <v>1144</v>
+      </c>
+      <c r="K84" s="29" t="s">
+        <v>1145</v>
+      </c>
+      <c r="L84" s="29" t="s">
+        <v>1146</v>
+      </c>
+      <c r="M84" s="29" t="s">
+        <v>1147</v>
+      </c>
+      <c r="N84" s="29" t="s">
+        <v>1154</v>
+      </c>
+      <c r="O84" s="29" t="s">
+        <v>1155</v>
+      </c>
+      <c r="P84" s="29" t="s">
+        <v>1156</v>
+      </c>
+      <c r="Q84" s="29" t="s">
+        <v>1157</v>
+      </c>
+      <c r="R84" s="29" t="s">
+        <v>1158</v>
+      </c>
+      <c r="S84" s="29" t="s">
+        <v>1159</v>
+      </c>
+      <c r="T84" s="29" t="s">
+        <v>1160</v>
+      </c>
+      <c r="U84" s="29" t="s">
+        <v>1161</v>
+      </c>
+      <c r="V84" s="29" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="F85" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="H85" s="29" t="s">
+        <v>1163</v>
+      </c>
+      <c r="I85" s="29" t="s">
+        <v>1164</v>
+      </c>
+      <c r="J85" s="29" t="s">
+        <v>1165</v>
+      </c>
+      <c r="K85" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="L85" s="29" t="s">
+        <v>1167</v>
+      </c>
+      <c r="M85" s="29" t="s">
+        <v>1168</v>
+      </c>
+      <c r="N85" s="29" t="s">
+        <v>1169</v>
+      </c>
+      <c r="O85" s="29" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C86" s="29" t="s">
         <v>733</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F86" s="4" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="29">
+      <c r="H86" s="29" t="s">
+        <v>1180</v>
+      </c>
+      <c r="I86" s="29" t="s">
+        <v>1181</v>
+      </c>
+      <c r="J86" s="29" t="s">
+        <v>1182</v>
+      </c>
+      <c r="K86" s="29" t="s">
+        <v>1183</v>
+      </c>
+      <c r="L86" s="29" t="s">
+        <v>1184</v>
+      </c>
+      <c r="M86" s="29" t="s">
+        <v>1185</v>
+      </c>
+      <c r="N86" s="29" t="s">
+        <v>1186</v>
+      </c>
+      <c r="O86" s="29" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A88" s="29">
         <v>11.4</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E88" s="4" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="88" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E88" s="4" t="s">
+    <row r="89" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E89" s="4" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E89" s="4" t="s">
+    <row r="90" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E90" s="4" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="90" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E90" s="4" t="s">
+    <row r="91" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E91" s="4" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="91" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E91" s="4" t="s">
+    <row r="92" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E92" s="4" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E92" s="4" t="s">
+    <row r="93" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E93" s="4" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="93" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A93" s="29">
+    <row r="94" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A94" s="29">
         <v>11.5</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C94" s="4" t="s">
         <v>756</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>757</v>
-      </c>
-      <c r="G93" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="H93" s="45" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="C94" s="4" t="s">
-        <v>761</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>757</v>
       </c>
+      <c r="G94" s="29" t="s">
+        <v>399</v>
+      </c>
       <c r="H94" s="45" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="C95" s="4" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>757</v>
       </c>
-      <c r="G95" s="29" t="s">
-        <v>399</v>
-      </c>
       <c r="H95" s="45" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C96" s="4" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>757</v>
@@ -14663,34 +14933,34 @@
         <v>399</v>
       </c>
       <c r="H96" s="45" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="97" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C97" s="6" t="s">
+      <c r="C97" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="G97" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="H97" s="45" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C98" s="6" t="s">
         <v>906</v>
       </c>
-      <c r="D97" s="6" t="s">
+      <c r="D98" s="6" t="s">
         <v>757</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C98" s="4" t="s">
-        <v>760</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>757</v>
-      </c>
-      <c r="G98" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="H98" s="45" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="99" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C99" s="4" t="s">
-        <v>907</v>
+        <v>760</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>757</v>
@@ -14699,115 +14969,106 @@
         <v>399</v>
       </c>
       <c r="H99" s="45" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C100" s="4" t="s">
+        <v>907</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="G100" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="H100" s="45" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I100" s="45" t="s">
         <v>1058</v>
       </c>
-      <c r="I99" s="45" t="s">
+      <c r="J100" s="45" t="s">
         <v>1059</v>
       </c>
-      <c r="J99" s="45" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A101" s="29">
+    </row>
+    <row r="101" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A102" s="29">
         <v>11.6</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>762</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>763</v>
-      </c>
-      <c r="G101" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="H101" s="45" t="s">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C102" s="4" t="s">
         <v>762</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G102" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H102" s="45" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A104" s="29">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C103" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="G103" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="H103" s="45" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A105" s="29">
         <v>11.7</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>764</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>757</v>
-      </c>
-      <c r="G104" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="H104" s="45" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C105" s="4" t="s">
         <v>764</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="G105" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H105" s="45" t="s">
-        <v>1062</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="106" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
+      <c r="C106" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="G106" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="H106" s="45" t="s">
+        <v>1061</v>
+      </c>
     </row>
     <row r="107" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A107" s="29">
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+    </row>
+    <row r="108" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A108" s="29">
         <v>11.8</v>
       </c>
-      <c r="C107" s="6" t="s">
+      <c r="C108" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="D107" s="6" t="s">
+      <c r="D108" s="6" t="s">
         <v>766</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C108" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>767</v>
-      </c>
-      <c r="G108" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="H108" s="45" t="s">
-        <v>1063</v>
-      </c>
-      <c r="I108" s="45" t="s">
-        <v>1064</v>
-      </c>
-      <c r="J108" s="45" t="s">
-        <v>1065</v>
-      </c>
-      <c r="K108" s="45" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="109" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14815,107 +15076,113 @@
         <v>263</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G109" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H109" s="45" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A111" s="29">
+        <v>1062</v>
+      </c>
+      <c r="I109" s="45" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J109" s="45" t="s">
+        <v>1064</v>
+      </c>
+      <c r="K109" s="45" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C110" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>768</v>
+      </c>
+      <c r="G110" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="H110" s="45" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A112" s="29">
         <v>11.9</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C112" s="4" t="s">
         <v>769</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>770</v>
-      </c>
-      <c r="G111" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="H111" s="45" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C112" s="4" t="s">
-        <v>378</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>770</v>
       </c>
+      <c r="G112" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="H112" s="45" t="s">
+        <v>1068</v>
+      </c>
     </row>
     <row r="113" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C113" s="3" t="s">
-        <v>502</v>
+      <c r="C113" s="4" t="s">
+        <v>378</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="G113" s="29" t="s">
+    </row>
+    <row r="114" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C114" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="G114" s="29" t="s">
         <v>399</v>
       </c>
-      <c r="H113" s="45" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="114" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
+      <c r="H114" s="45" t="s">
+        <v>1067</v>
+      </c>
     </row>
     <row r="115" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="1:16" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A116" s="31">
+    <row r="116" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+    </row>
+    <row r="117" spans="1:16" s="29" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A117" s="31">
         <v>11.1</v>
       </c>
-      <c r="C116" s="4" t="s">
-        <v>771</v>
-      </c>
-      <c r="D116" s="4" t="s">
-        <v>772</v>
-      </c>
-      <c r="G116" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="H116" s="44" t="s">
-        <v>1074</v>
-      </c>
-      <c r="I116" s="44" t="s">
-        <v>1070</v>
-      </c>
-      <c r="J116" s="44" t="s">
-        <v>1071</v>
-      </c>
-      <c r="K116" s="44" t="s">
-        <v>1072</v>
-      </c>
-      <c r="L116" s="44" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="117" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C117" s="4" t="s">
         <v>771</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G117" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H117" s="44" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="I117" s="44" t="s">
-        <v>1076</v>
+        <v>1069</v>
+      </c>
+      <c r="J117" s="44" t="s">
+        <v>1070</v>
+      </c>
+      <c r="K117" s="44" t="s">
+        <v>1071</v>
+      </c>
+      <c r="L117" s="44" t="s">
+        <v>1072</v>
       </c>
     </row>
     <row r="118" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14923,13 +15190,16 @@
         <v>771</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G118" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H118" s="44" t="s">
-        <v>1077</v>
+        <v>1074</v>
+      </c>
+      <c r="I118" s="44" t="s">
+        <v>1075</v>
       </c>
     </row>
     <row r="119" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -14937,149 +15207,146 @@
         <v>771</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="G119" s="29" t="s">
         <v>399</v>
       </c>
       <c r="H119" s="44" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C120" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="G120" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="H120" s="44" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I120" s="44" t="s">
         <v>1078</v>
       </c>
-      <c r="I119" s="44" t="s">
+      <c r="J120" s="44" t="s">
         <v>1079</v>
       </c>
-      <c r="J119" s="44" t="s">
+      <c r="K120" s="44" t="s">
         <v>1080</v>
       </c>
-      <c r="K119" s="44" t="s">
+      <c r="L120" s="44" t="s">
         <v>1081</v>
       </c>
-      <c r="L119" s="44" t="s">
+      <c r="M120" s="44" t="s">
         <v>1082</v>
       </c>
-      <c r="M119" s="44" t="s">
+      <c r="N120" s="44" t="s">
         <v>1083</v>
       </c>
-      <c r="N119" s="44" t="s">
+      <c r="O120" s="44" t="s">
         <v>1084</v>
       </c>
-      <c r="O119" s="44" t="s">
+      <c r="P120" s="44" t="s">
         <v>1085</v>
-      </c>
-      <c r="P119" s="44" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="120" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="H120" s="44" t="s">
-        <v>1025</v>
-      </c>
-      <c r="I120" s="44" t="s">
-        <v>1087</v>
-      </c>
-      <c r="J120" s="44" t="s">
-        <v>1088</v>
-      </c>
-      <c r="K120" s="44" t="s">
-        <v>1089</v>
-      </c>
-      <c r="L120" s="44" t="s">
-        <v>1090</v>
-      </c>
-      <c r="M120" s="44" t="s">
-        <v>962</v>
-      </c>
-      <c r="N120" s="44" t="s">
-        <v>1091</v>
-      </c>
-      <c r="O120" s="44" t="s">
-        <v>1092</v>
-      </c>
-      <c r="P120" s="44" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="121" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="H121" s="44" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I121" s="44" t="s">
+        <v>1086</v>
+      </c>
+      <c r="J121" s="44" t="s">
+        <v>1087</v>
+      </c>
+      <c r="K121" s="44" t="s">
+        <v>1088</v>
+      </c>
+      <c r="L121" s="44" t="s">
+        <v>1089</v>
+      </c>
+      <c r="M121" s="44" t="s">
+        <v>962</v>
+      </c>
+      <c r="N121" s="44" t="s">
+        <v>1090</v>
+      </c>
+      <c r="O121" s="44" t="s">
+        <v>1091</v>
+      </c>
+      <c r="P121" s="44" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H122" s="44" t="s">
+        <v>1093</v>
+      </c>
+      <c r="I122" s="44" t="s">
         <v>1094</v>
       </c>
-      <c r="I121" s="44" t="s">
+      <c r="J122" s="44" t="s">
         <v>1095</v>
       </c>
-      <c r="J121" s="44" t="s">
+      <c r="K122" s="44" t="s">
         <v>1096</v>
       </c>
-      <c r="K121" s="44" t="s">
+      <c r="L122" s="44" t="s">
         <v>1097</v>
       </c>
-      <c r="L121" s="44" t="s">
+      <c r="M122" s="44" t="s">
         <v>1098</v>
       </c>
-      <c r="M121" s="44" t="s">
+      <c r="N122" s="44" t="s">
         <v>1099</v>
       </c>
-      <c r="N121" s="44" t="s">
+      <c r="O122" s="44" t="s">
         <v>1100</v>
       </c>
-      <c r="O121" s="44" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A123" s="29">
-        <v>11.11</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>776</v>
-      </c>
-      <c r="D123" s="4" t="s">
-        <v>775</v>
-      </c>
-      <c r="H123" s="44" t="s">
-        <v>1102</v>
-      </c>
-      <c r="I123" s="44" t="s">
-        <v>1103</v>
-      </c>
-      <c r="J123" s="44" t="s">
-        <v>1104</v>
-      </c>
-      <c r="K123" s="44" t="s">
-        <v>1105</v>
-      </c>
-      <c r="L123" s="44" t="s">
-        <v>1106</v>
-      </c>
-    </row>
+    </row>
+    <row r="123" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="124" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A124" s="29">
-        <v>11.12</v>
+        <v>11.11</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>776</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="H124" s="44" t="s">
-        <v>1110</v>
+        <v>1101</v>
+      </c>
+      <c r="I124" s="44" t="s">
+        <v>1102</v>
+      </c>
+      <c r="J124" s="44" t="s">
+        <v>1103</v>
+      </c>
+      <c r="K124" s="44" t="s">
+        <v>1104</v>
+      </c>
+      <c r="L124" s="44" t="s">
+        <v>1105</v>
       </c>
     </row>
     <row r="125" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A125" s="29">
+        <v>11.12</v>
+      </c>
       <c r="C125" s="4" t="s">
         <v>776</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="H125" s="44" t="s">
-        <v>1107</v>
-      </c>
-      <c r="I125" s="43" t="s">
-        <v>1108</v>
-      </c>
-      <c r="J125" s="43" t="s">
         <v>1109</v>
       </c>
     </row>
@@ -15088,54 +15355,45 @@
         <v>776</v>
       </c>
       <c r="D126" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="H126" s="44" t="s">
+        <v>1106</v>
+      </c>
+      <c r="I126" s="43" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J126" s="43" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C127" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="D127" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="H126" s="44" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:16" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A128" s="29">
+      <c r="H127" s="44" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A129" s="29">
         <v>11.13</v>
       </c>
-      <c r="C128" s="4" t="s">
-        <v>780</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>781</v>
-      </c>
-      <c r="H128" s="44" t="s">
-        <v>1112</v>
-      </c>
-      <c r="I128" s="44" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C129" s="4" t="s">
         <v>780</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>416</v>
+        <v>781</v>
       </c>
       <c r="H129" s="44" t="s">
-        <v>1114</v>
-      </c>
-      <c r="I129" s="43" t="s">
-        <v>925</v>
-      </c>
-      <c r="J129" s="44" t="s">
-        <v>951</v>
-      </c>
-      <c r="K129" s="44" t="s">
-        <v>1115</v>
-      </c>
-      <c r="L129" s="43" t="s">
-        <v>1116</v>
-      </c>
-      <c r="M129" s="29" t="s">
-        <v>988</v>
+        <v>1111</v>
+      </c>
+      <c r="I129" s="44" t="s">
+        <v>1112</v>
       </c>
     </row>
     <row r="130" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15143,44 +15401,56 @@
         <v>780</v>
       </c>
       <c r="D130" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="H130" s="44" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I130" s="43" t="s">
+        <v>925</v>
+      </c>
+      <c r="J130" s="44" t="s">
+        <v>951</v>
+      </c>
+      <c r="K130" s="44" t="s">
+        <v>1114</v>
+      </c>
+      <c r="L130" s="43" t="s">
+        <v>1115</v>
+      </c>
+      <c r="M130" s="29" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C131" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="D131" s="4" t="s">
         <v>782</v>
       </c>
-      <c r="H130" s="44" t="s">
+      <c r="H131" s="44" t="s">
+        <v>1116</v>
+      </c>
+      <c r="I131" s="44" t="s">
         <v>1117</v>
       </c>
-      <c r="I130" s="44" t="s">
+    </row>
+    <row r="132" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C132" s="32" t="s">
+        <v>780</v>
+      </c>
+      <c r="D132" s="32" t="s">
+        <v>783</v>
+      </c>
+      <c r="H132" s="44" t="s">
         <v>1118</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C131" s="32" t="s">
-        <v>780</v>
-      </c>
-      <c r="D131" s="32" t="s">
-        <v>783</v>
-      </c>
-      <c r="H131" s="44" t="s">
+      <c r="I132" s="44" t="s">
         <v>1119</v>
       </c>
-      <c r="I131" s="44" t="s">
+      <c r="J132" s="44" t="s">
         <v>1120</v>
-      </c>
-      <c r="J131" s="44" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C132" s="4" t="s">
-        <v>780</v>
-      </c>
-      <c r="D132" s="4" t="s">
-        <v>784</v>
-      </c>
-      <c r="H132" s="44" t="s">
-        <v>1068</v>
-      </c>
-      <c r="I132" s="44" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="133" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15188,13 +15458,13 @@
         <v>780</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H133" s="44" t="s">
-        <v>953</v>
+        <v>1067</v>
       </c>
       <c r="I133" s="44" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="134" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15202,364 +15472,379 @@
         <v>780</v>
       </c>
       <c r="D134" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="H134" s="44" t="s">
+        <v>953</v>
+      </c>
+      <c r="I134" s="44" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C135" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="D135" s="4" t="s">
         <v>786</v>
       </c>
-      <c r="H134" s="46" t="s">
+      <c r="H135" s="46" t="s">
+        <v>1123</v>
+      </c>
+      <c r="I135" s="46" t="s">
         <v>1124</v>
       </c>
-      <c r="I134" s="46" t="s">
+      <c r="J135" s="46" t="s">
         <v>1125</v>
       </c>
-      <c r="J134" s="46" t="s">
+      <c r="K135" s="46" t="s">
         <v>1126</v>
       </c>
-      <c r="K134" s="46" t="s">
+      <c r="L135" s="43" t="s">
         <v>1127</v>
       </c>
-      <c r="L134" s="43" t="s">
+      <c r="M135" s="46" t="s">
         <v>1128</v>
       </c>
-      <c r="M134" s="46" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A136" s="29">
+    </row>
+    <row r="136" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A137" s="29">
         <v>11.14</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="C137" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="D136" s="4" t="s">
+      <c r="D137" s="4" t="s">
         <v>787</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C137" s="4"/>
-      <c r="D137" s="4" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="138" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C138" s="4"/>
       <c r="D138" s="4" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C139" s="4"/>
+      <c r="D139" s="4" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="139" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A140" s="29">
+    <row r="140" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A141" s="29">
         <v>11.15</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="C141" s="4" t="s">
         <v>790</v>
-      </c>
-      <c r="D140" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="H140" s="44" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C141" s="4" t="s">
-        <v>791</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>416</v>
       </c>
       <c r="H141" s="44" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A143" s="29">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C142" s="4" t="s">
+        <v>791</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="H142" s="44" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A144" s="29">
         <v>11.16</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D144" s="4" t="s">
         <v>792</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D144" s="4" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="145" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D145" s="4" t="s">
-        <v>793</v>
+        <v>813</v>
       </c>
     </row>
     <row r="146" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D146" s="4" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="147" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D147" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="148" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D148" s="4" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="149" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D149" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="150" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D150" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="151" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D151" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="152" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D152" s="4" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="153" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D153" s="4" t="s">
-        <v>908</v>
+        <v>800</v>
       </c>
     </row>
     <row r="154" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D154" s="4" t="s">
-        <v>801</v>
+        <v>908</v>
       </c>
     </row>
     <row r="155" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D155" s="4" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="156" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D156" s="4" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D157" s="4" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="157" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D157" s="32" t="s">
-        <v>1132</v>
-      </c>
-    </row>
     <row r="158" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D158" s="4" t="s">
-        <v>804</v>
+      <c r="D158" s="32" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="159" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D159" s="4" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="160" spans="4:4" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D160" s="4" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="161" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D161" s="4" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
     </row>
     <row r="162" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D162" s="4" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D163" s="4" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="163" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D163" s="32" t="s">
+    <row r="164" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D164" s="32" t="s">
         <v>808</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D164" s="4" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="165" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D165" s="4" t="s">
-        <v>815</v>
+        <v>892</v>
       </c>
     </row>
     <row r="166" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D166" s="4" t="s">
-        <v>809</v>
+        <v>815</v>
       </c>
     </row>
     <row r="167" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D167" s="4" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="168" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D168" s="4" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" s="29" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D169" s="4" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D169" s="4" t="s">
+    <row r="170" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D170" s="4" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="171" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A171" s="4">
+    <row r="172" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A172" s="4">
         <v>11.17</v>
       </c>
-      <c r="E171" s="4" t="s">
+      <c r="E172" s="4" t="s">
         <v>816</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E172" s="4" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E173" s="4" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E174" s="4" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E175" s="4" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E176" s="4" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="177" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E177" s="4" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="178" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E178" s="4" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="179" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E179" s="4" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="180" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E180" s="4" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="181" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E181" s="4" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="182" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E182" s="4" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="183" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E183" s="4" t="s">
-        <v>893</v>
+        <v>827</v>
       </c>
     </row>
     <row r="184" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E184" s="4" t="s">
-        <v>828</v>
+        <v>893</v>
       </c>
     </row>
     <row r="185" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E185" s="4" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="186" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E186" s="4" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="187" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E187" s="4" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="188" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E188" s="4" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="189" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E189" s="4" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="190" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E190" s="4" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
     </row>
     <row r="191" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E191" s="4" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
     </row>
     <row r="192" spans="5:5" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E192" s="4" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="193" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E193" s="4" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="194" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E194" s="4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="195" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E195" s="4" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E196" s="4" t="s">
         <v>838</v>
       </c>
     </row>
-    <row r="196" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A196" s="4">
+    <row r="197" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A197" s="4">
         <v>11.18</v>
       </c>
-      <c r="C196" s="4" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F196" s="4" t="s">
+      <c r="C197" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F197" s="4" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="197" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="198" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="199" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="200" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="201" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="202" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="203" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="204" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TS 2,3 TSPP 2.1 Tamil files 13/05/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -11487,8 +11487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D75" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="M68" sqref="M68"/>
@@ -13925,7 +13925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="E69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>

</xml_diff>